<commit_message>
fixed beer table price reading, removed tap beer category as its dumb.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://theartsyndicate.sharepoint.com/sites/TheArtSyndicte/Shared Documents/Assets/SRC/Autoscript/TheArtSyndicateMenu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB343A4E-E2FE-4D5B-9176-F77F52434506}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF0C5627-0AA8-4627-907E-157B77F65BAB}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="3110" windowWidth="14400" windowHeight="8170" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="266">
   <si>
     <t>Chapter</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t xml:space="preserve">"Andy Smash" Hazy Pale Ale </t>
-  </si>
-  <si>
-    <t>"Dolly Aldrin" Yuzu Berliner Weisse</t>
   </si>
   <si>
     <t>Alexandria, Sydney</t>
@@ -832,6 +829,15 @@
   <si>
     <t>Seven Spice</t>
   </si>
+  <si>
+    <t>"Dolly Aldrin" Yuzu Berliner Weisse</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>Ask about our latest tap beers, or just look at our tap.</t>
+  </si>
 </sst>
 </file>
 
@@ -970,7 +976,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1167,6 +1173,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1734,7 +1743,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AA1063" headerRowCount="0" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AA1064" headerRowCount="0" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34">
   <tableColumns count="27">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="33"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="32"/>
@@ -2062,12 +2071,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1063"/>
+  <dimension ref="A1:AA1064"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2149,22 +2158,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>186</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
@@ -2247,20 +2256,20 @@
         <v>2022</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>37</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -2341,20 +2350,20 @@
         <v>2023</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="I6" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>209</v>
-      </c>
       <c r="J6" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
@@ -2388,20 +2397,20 @@
         <v>2021</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" s="17" t="s">
         <v>193</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>194</v>
       </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -2435,22 +2444,22 @@
         <v>2023</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>37</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -2496,7 +2505,7 @@
         <v>41</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>42</v>
@@ -2533,22 +2542,22 @@
         <v>2014</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
@@ -2570,7 +2579,7 @@
     </row>
     <row r="11" spans="1:27" s="35" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="32">
         <v>17</v>
@@ -2582,22 +2591,22 @@
         <v>2021</v>
       </c>
       <c r="E11" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="G11" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="H11" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="H11" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>219</v>
-      </c>
       <c r="J11" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
@@ -2619,7 +2628,7 @@
     </row>
     <row r="12" spans="1:27" s="31" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="27">
         <v>14</v>
@@ -2631,22 +2640,22 @@
         <v>2023</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F12" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="H12" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="J12" s="15" t="s">
         <v>204</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>203</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
@@ -2668,7 +2677,7 @@
     </row>
     <row r="13" spans="1:27" s="31" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B13" s="27">
         <v>17</v>
@@ -2680,22 +2689,22 @@
         <v>2022</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
@@ -2729,22 +2738,22 @@
         <v>2023</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
@@ -2781,19 +2790,19 @@
         <v>44</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H15" s="33" t="s">
         <v>46</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
@@ -2827,22 +2836,22 @@
         <v>2022</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G16" s="28" t="s">
         <v>48</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I16" s="29" t="s">
         <v>31</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
@@ -2875,20 +2884,20 @@
         <v>2023</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F17" s="63"/>
       <c r="G17" s="62" t="s">
+        <v>243</v>
+      </c>
+      <c r="H17" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="I17" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="J17" s="22" t="s">
         <v>246</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>247</v>
       </c>
       <c r="K17" s="65"/>
       <c r="L17" s="65"/>
@@ -2922,11 +2931,11 @@
         <v>2021</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>56</v>
@@ -2935,7 +2944,7 @@
         <v>57</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -2969,22 +2978,22 @@
         <v>2017</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>49</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I19" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -3033,7 +3042,7 @@
         <v>54</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
@@ -3067,22 +3076,22 @@
         <v>2022</v>
       </c>
       <c r="E21" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="F21" s="28" t="s">
-        <v>153</v>
-      </c>
       <c r="G21" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I21" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -3151,46 +3160,42 @@
       <c r="Z22" s="30"/>
       <c r="AA22" s="30"/>
     </row>
-    <row r="23" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="44">
-        <v>13</v>
-      </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
+      <c r="B23" s="67">
+        <v>9.5</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="30"/>
     </row>
     <row r="24" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
@@ -3204,8 +3209,8 @@
       <c r="E24" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="44" t="s">
-        <v>69</v>
+      <c r="F24" s="47" t="s">
+        <v>67</v>
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="48"/>
@@ -3233,7 +3238,7 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
-    <row r="25" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>65</v>
       </c>
@@ -3243,17 +3248,15 @@
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
       <c r="E25" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="50" t="s">
-        <v>211</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="44"/>
       <c r="H25" s="48"/>
       <c r="I25" s="44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>64</v>
@@ -3276,25 +3279,27 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
     </row>
-    <row r="26" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="44">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
       <c r="E26" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F26" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="46"/>
+        <v>263</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>210</v>
+      </c>
       <c r="H26" s="48"/>
       <c r="I26" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>64</v>
@@ -3317,135 +3322,145 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:27" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="44">
+        <v>12</v>
+      </c>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+    </row>
+    <row r="28" spans="1:27" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="37">
         <v>15</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="F27" s="51" t="s">
+      <c r="G28" s="51"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="19"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+    </row>
+    <row r="29" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="32">
+        <v>13</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="51"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37" t="s">
+      <c r="G29" s="36"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="52"/>
-      <c r="S27" s="52"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="52"/>
-      <c r="Y27" s="52"/>
-      <c r="Z27" s="52"/>
-      <c r="AA27" s="52"/>
-    </row>
-    <row r="28" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="J29" s="21"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+    </row>
+    <row r="30" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="32">
-        <v>13</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="34"/>
-      <c r="W28" s="34"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="34"/>
-    </row>
-    <row r="29" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="44">
+      <c r="B30" s="44">
         <v>10</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-    </row>
-    <row r="30" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
+      <c r="E30" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>73</v>
+      </c>
       <c r="G30" s="46"/>
       <c r="H30" s="48"/>
-      <c r="I30" s="44"/>
+      <c r="I30" s="44" t="s">
+        <v>74</v>
+      </c>
       <c r="J30" s="4" t="s">
         <v>64</v>
       </c>
@@ -3467,22 +3482,14 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
     </row>
-    <row r="31" spans="1:27" ht="29" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="44">
-        <v>22</v>
-      </c>
+    <row r="31" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="46"/>
       <c r="D31" s="46"/>
       <c r="E31" s="46"/>
-      <c r="F31" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="54" t="s">
-        <v>249</v>
-      </c>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="48"/>
       <c r="I31" s="44"/>
       <c r="J31" s="4" t="s">
@@ -3506,21 +3513,21 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
     </row>
-    <row r="32" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="44">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="46"/>
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
-      <c r="F32" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G32" s="46" t="s">
-        <v>79</v>
+      <c r="F32" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>248</v>
       </c>
       <c r="H32" s="48"/>
       <c r="I32" s="44"/>
@@ -3547,19 +3554,19 @@
     </row>
     <row r="33" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="44">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
       <c r="F33" s="46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G33" s="46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H33" s="48"/>
       <c r="I33" s="44"/>
@@ -3586,18 +3593,20 @@
     </row>
     <row r="34" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="44">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C34" s="46"/>
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="G34" s="46"/>
+        <v>79</v>
+      </c>
+      <c r="G34" s="46" t="s">
+        <v>80</v>
+      </c>
       <c r="H34" s="48"/>
       <c r="I34" s="44"/>
       <c r="J34" s="4" t="s">
@@ -3623,16 +3632,16 @@
     </row>
     <row r="35" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="44">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="46"/>
       <c r="D35" s="46"/>
       <c r="E35" s="46"/>
       <c r="F35" s="46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G35" s="46"/>
       <c r="H35" s="48"/>
@@ -3658,135 +3667,133 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="32">
+    <row r="36" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="44">
+        <v>20</v>
+      </c>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="46"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+    </row>
+    <row r="37" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="32">
         <v>12</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="G36" s="36" t="s">
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="G37" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="34"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="34"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="34"/>
+      <c r="AA37" s="34"/>
+    </row>
+    <row r="38" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="44">
+        <v>24</v>
+      </c>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="21" t="s">
+      <c r="G38" s="46"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
-    </row>
-    <row r="37" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="44">
-        <v>24</v>
-      </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="46"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5"/>
-    </row>
-    <row r="38" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="32">
-        <v>22</v>
-      </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="G38" s="32"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="34"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="34"/>
-      <c r="W38" s="34"/>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="34"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="34"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
     </row>
     <row r="39" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B39" s="32">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C39" s="36"/>
       <c r="D39" s="36"/>
       <c r="E39" s="36"/>
       <c r="F39" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>230</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="G39" s="32"/>
       <c r="H39" s="33"/>
       <c r="I39" s="32"/>
       <c r="J39" s="21" t="s">
@@ -3812,23 +3819,25 @@
     </row>
     <row r="40" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="32">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
       <c r="E40" s="36"/>
       <c r="F40" s="36" t="s">
-        <v>228</v>
+        <v>86</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H40" s="33"/>
       <c r="I40" s="32"/>
-      <c r="J40" s="21"/>
+      <c r="J40" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
@@ -3849,19 +3858,19 @@
     </row>
     <row r="41" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" s="32">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="G41" s="36" t="s">
         <v>229</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>230</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="32"/>
@@ -3884,122 +3893,118 @@
       <c r="Z41" s="34"/>
       <c r="AA41" s="34"/>
     </row>
-    <row r="42" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="4" t="s">
+    <row r="42" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="32">
+        <v>12</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="H42" s="33"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
+      <c r="T42" s="34"/>
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="34"/>
+      <c r="X42" s="34"/>
+      <c r="Y42" s="34"/>
+      <c r="Z42" s="34"/>
+      <c r="AA42" s="34"/>
+    </row>
+    <row r="43" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5"/>
-    </row>
-    <row r="43" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+    </row>
+    <row r="44" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="32">
+        <v>10</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="32">
-        <v>10</v>
-      </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36" t="s">
+      <c r="G44" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="H44" s="33"/>
+      <c r="I44" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H43" s="33"/>
-      <c r="I43" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="J43" s="21" t="s">
+      <c r="J44" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="34"/>
-      <c r="P43" s="34"/>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="34"/>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
-      <c r="U43" s="34"/>
-      <c r="V43" s="34"/>
-      <c r="W43" s="34"/>
-      <c r="X43" s="34"/>
-      <c r="Y43" s="34"/>
-      <c r="Z43" s="34"/>
-      <c r="AA43" s="34"/>
-    </row>
-    <row r="44" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="44">
-        <v>13</v>
-      </c>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="H44" s="48"/>
-      <c r="I44" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
-      <c r="Y44" s="5"/>
-      <c r="Z44" s="5"/>
-      <c r="AA44" s="5"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
+      <c r="O44" s="34"/>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="34"/>
+      <c r="S44" s="34"/>
+      <c r="T44" s="34"/>
+      <c r="U44" s="34"/>
+      <c r="V44" s="34"/>
+      <c r="W44" s="34"/>
+      <c r="X44" s="34"/>
+      <c r="Y44" s="34"/>
+      <c r="Z44" s="34"/>
+      <c r="AA44" s="34"/>
     </row>
     <row r="45" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" s="44">
         <v>13</v>
@@ -4008,14 +4013,14 @@
       <c r="D45" s="46"/>
       <c r="E45" s="46"/>
       <c r="F45" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G45" s="46" t="s">
         <v>262</v>
       </c>
       <c r="H45" s="48"/>
       <c r="I45" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>64</v>
@@ -4038,189 +4043,189 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="32">
+    <row r="46" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="44">
+        <v>13</v>
+      </c>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="G46" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="H46" s="48"/>
+      <c r="I46" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+    </row>
+    <row r="47" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="32">
         <v>14</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36" t="s">
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="H47" s="33"/>
+      <c r="I47" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G46" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="H46" s="33"/>
-      <c r="I46" s="32" t="s">
+      <c r="J47" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="34"/>
+      <c r="P47" s="34"/>
+      <c r="Q47" s="34"/>
+      <c r="R47" s="34"/>
+      <c r="S47" s="34"/>
+      <c r="T47" s="34"/>
+      <c r="U47" s="34"/>
+      <c r="V47" s="34"/>
+      <c r="W47" s="34"/>
+      <c r="X47" s="34"/>
+      <c r="Y47" s="34"/>
+      <c r="Z47" s="34"/>
+      <c r="AA47" s="34"/>
+    </row>
+    <row r="48" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="48">
+        <v>16</v>
+      </c>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="J46" s="21" t="s">
+      <c r="G48" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="H48" s="48"/>
+      <c r="I48" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="34"/>
-      <c r="T46" s="34"/>
-      <c r="U46" s="34"/>
-      <c r="V46" s="34"/>
-      <c r="W46" s="34"/>
-      <c r="X46" s="34"/>
-      <c r="Y46" s="34"/>
-      <c r="Z46" s="34"/>
-      <c r="AA46" s="34"/>
-    </row>
-    <row r="47" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="48">
-        <v>16</v>
-      </c>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="48"/>
-      <c r="I47" s="44" t="s">
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+    </row>
+    <row r="49" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="B49" s="27">
+        <v>10</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="H49" s="29"/>
+      <c r="I49" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="J49" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-    </row>
-    <row r="48" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="27">
-        <v>10</v>
-      </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H48" s="29"/>
-      <c r="I48" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
-      <c r="S48" s="30"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="30"/>
-      <c r="V48" s="30"/>
-      <c r="W48" s="30"/>
-      <c r="X48" s="30"/>
-      <c r="Y48" s="30"/>
-      <c r="Z48" s="30"/>
-      <c r="AA48" s="30"/>
-    </row>
-    <row r="49" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" s="44">
-        <v>10.5</v>
-      </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="H49" s="48"/>
-      <c r="I49" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
-      <c r="Y49" s="5"/>
-      <c r="Z49" s="5"/>
-      <c r="AA49" s="5"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="30"/>
+      <c r="N49" s="30"/>
+      <c r="O49" s="30"/>
+      <c r="P49" s="30"/>
+      <c r="Q49" s="30"/>
+      <c r="R49" s="30"/>
+      <c r="S49" s="30"/>
+      <c r="T49" s="30"/>
+      <c r="U49" s="30"/>
+      <c r="V49" s="30"/>
+      <c r="W49" s="30"/>
+      <c r="X49" s="30"/>
+      <c r="Y49" s="30"/>
+      <c r="Z49" s="30"/>
+      <c r="AA49" s="30"/>
     </row>
     <row r="50" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="44">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="C50" s="46"/>
       <c r="D50" s="46"/>
       <c r="E50" s="46"/>
-      <c r="F50" s="46" t="s">
-        <v>100</v>
+      <c r="F50" s="55" t="s">
+        <v>97</v>
       </c>
       <c r="G50" s="46" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H50" s="48"/>
       <c r="I50" s="44" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>64</v>
@@ -4243,27 +4248,29 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
     </row>
-    <row r="51" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B51" s="44">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" s="46"/>
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
       <c r="F51" s="46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G51" s="46" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H51" s="48"/>
       <c r="I51" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="J51" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
@@ -4282,29 +4289,27 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
     </row>
-    <row r="52" spans="1:27" ht="29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" s="44">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C52" s="46"/>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
       <c r="F52" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="G52" s="50" t="s">
-        <v>260</v>
+        <v>102</v>
+      </c>
+      <c r="G52" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="H52" s="48"/>
       <c r="I52" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="J52" s="4"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
@@ -4325,23 +4330,23 @@
     </row>
     <row r="53" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="44">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C53" s="46"/>
       <c r="D53" s="46"/>
       <c r="E53" s="46"/>
       <c r="F53" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G53" s="50" t="s">
         <v>259</v>
       </c>
       <c r="H53" s="48"/>
       <c r="I53" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>64</v>
@@ -4366,23 +4371,23 @@
     </row>
     <row r="54" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="44">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C54" s="46"/>
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
       <c r="F54" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G54" s="50" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="H54" s="48"/>
       <c r="I54" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>64</v>
@@ -4405,25 +4410,25 @@
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
     </row>
-    <row r="55" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="44">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C55" s="46"/>
       <c r="D55" s="46"/>
       <c r="E55" s="46"/>
       <c r="F55" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="G55" s="46" t="s">
-        <v>108</v>
+        <v>93</v>
+      </c>
+      <c r="G55" s="50" t="s">
+        <v>105</v>
       </c>
       <c r="H55" s="48"/>
       <c r="I55" s="44" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>64</v>
@@ -4448,23 +4453,23 @@
     </row>
     <row r="56" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="44">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C56" s="46"/>
       <c r="D56" s="46"/>
       <c r="E56" s="46"/>
       <c r="F56" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G56" s="46" t="s">
         <v>107</v>
-      </c>
-      <c r="G56" s="46" t="s">
-        <v>110</v>
       </c>
       <c r="H56" s="48"/>
       <c r="I56" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>64</v>
@@ -4489,23 +4494,23 @@
     </row>
     <row r="57" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B57" s="44">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C57" s="46"/>
       <c r="D57" s="46"/>
       <c r="E57" s="46"/>
       <c r="F57" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G57" s="46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H57" s="48"/>
       <c r="I57" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>64</v>
@@ -4530,23 +4535,23 @@
     </row>
     <row r="58" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B58" s="44">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C58" s="46"/>
       <c r="D58" s="46"/>
       <c r="E58" s="46"/>
       <c r="F58" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G58" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H58" s="48"/>
       <c r="I58" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>64</v>
@@ -4571,23 +4576,23 @@
     </row>
     <row r="59" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B59" s="44">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C59" s="46"/>
       <c r="D59" s="46"/>
       <c r="E59" s="46"/>
       <c r="F59" s="46" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G59" s="46" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H59" s="48"/>
       <c r="I59" s="44" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>64</v>
@@ -4612,23 +4617,23 @@
     </row>
     <row r="60" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B60" s="44">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C60" s="46"/>
       <c r="D60" s="46"/>
       <c r="E60" s="46"/>
       <c r="F60" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" s="46" t="s">
         <v>114</v>
-      </c>
-      <c r="G60" s="46" t="s">
-        <v>117</v>
       </c>
       <c r="H60" s="48"/>
       <c r="I60" s="44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>64</v>
@@ -4653,23 +4658,23 @@
     </row>
     <row r="61" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B61" s="44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" s="46"/>
       <c r="D61" s="46"/>
       <c r="E61" s="46"/>
       <c r="F61" s="46" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="G61" s="46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H61" s="48"/>
       <c r="I61" s="44" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>64</v>
@@ -4694,7 +4699,7 @@
     </row>
     <row r="62" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="44" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B62" s="44">
         <v>13</v>
@@ -4703,14 +4708,14 @@
       <c r="D62" s="46"/>
       <c r="E62" s="46"/>
       <c r="F62" s="46" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="G62" s="46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H62" s="48"/>
       <c r="I62" s="44" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>64</v>
@@ -4734,16 +4739,28 @@
       <c r="AA62" s="5"/>
     </row>
     <row r="63" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="44"/>
+      <c r="A63" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="44">
+        <v>13</v>
+      </c>
       <c r="C63" s="46"/>
       <c r="D63" s="46"/>
       <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
+      <c r="F63" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="G63" s="46" t="s">
+        <v>119</v>
+      </c>
       <c r="H63" s="48"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="4"/>
+      <c r="I63" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
@@ -4792,28 +4809,16 @@
       <c r="AA64" s="5"/>
     </row>
     <row r="65" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="B65" s="44">
-        <v>12</v>
-      </c>
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
       <c r="C65" s="46"/>
       <c r="D65" s="46"/>
       <c r="E65" s="46"/>
-      <c r="F65" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="G65" s="46" t="s">
-        <v>125</v>
-      </c>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
       <c r="H65" s="48"/>
-      <c r="I65" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="I65" s="44"/>
+      <c r="J65" s="4"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
@@ -4832,66 +4837,66 @@
       <c r="Z65" s="5"/>
       <c r="AA65" s="5"/>
     </row>
-    <row r="66" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B66" s="32">
-        <v>8</v>
-      </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="G66" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="H66" s="33"/>
-      <c r="I66" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="J66" s="21" t="s">
+    <row r="66" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="44">
+        <v>12</v>
+      </c>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G66" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H66" s="48"/>
+      <c r="I66" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
-      <c r="M66" s="34"/>
-      <c r="N66" s="34"/>
-      <c r="O66" s="34"/>
-      <c r="P66" s="34"/>
-      <c r="Q66" s="34"/>
-      <c r="R66" s="34"/>
-      <c r="S66" s="34"/>
-      <c r="T66" s="34"/>
-      <c r="U66" s="34"/>
-      <c r="V66" s="34"/>
-      <c r="W66" s="34"/>
-      <c r="X66" s="34"/>
-      <c r="Y66" s="34"/>
-      <c r="Z66" s="34"/>
-      <c r="AA66" s="34"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+      <c r="AA66" s="5"/>
     </row>
     <row r="67" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="32">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" s="36"/>
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
       <c r="F67" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="G67" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="G67" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="32" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="J67" s="21" t="s">
         <v>64</v>
@@ -4916,7 +4921,7 @@
     </row>
     <row r="68" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B68" s="32">
         <v>9</v>
@@ -4925,14 +4930,14 @@
       <c r="D68" s="36"/>
       <c r="E68" s="36"/>
       <c r="F68" s="36" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="G68" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H68" s="33"/>
       <c r="I68" s="32" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="J68" s="21" t="s">
         <v>64</v>
@@ -4955,87 +4960,89 @@
       <c r="Z68" s="34"/>
       <c r="AA68" s="34"/>
     </row>
-    <row r="69" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="44" t="s">
+    <row r="69" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" s="32">
+        <v>9</v>
+      </c>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="G69" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="H69" s="33"/>
+      <c r="I69" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J69" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K69" s="34"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="34"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34"/>
+      <c r="Q69" s="34"/>
+      <c r="R69" s="34"/>
+      <c r="S69" s="34"/>
+      <c r="T69" s="34"/>
+      <c r="U69" s="34"/>
+      <c r="V69" s="34"/>
+      <c r="W69" s="34"/>
+      <c r="X69" s="34"/>
+      <c r="Y69" s="34"/>
+      <c r="Z69" s="34"/>
+      <c r="AA69" s="34"/>
+    </row>
+    <row r="70" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B70" s="44">
+        <v>10</v>
+      </c>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="G70" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="44">
-        <v>10</v>
-      </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46" t="s">
+      <c r="H70" s="48"/>
+      <c r="I70" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="G69" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="H69" s="48"/>
-      <c r="I69" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="J69" s="4"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
-      <c r="Z69" s="5"/>
-      <c r="AA69" s="5"/>
-    </row>
-    <row r="70" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="B70" s="27">
-        <v>11</v>
-      </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G70" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J70" s="16"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="30"/>
-      <c r="M70" s="30"/>
-      <c r="N70" s="30"/>
-      <c r="O70" s="30"/>
-      <c r="P70" s="30"/>
-      <c r="Q70" s="30"/>
-      <c r="R70" s="30"/>
-      <c r="S70" s="30"/>
-      <c r="T70" s="30"/>
-      <c r="U70" s="30"/>
-      <c r="V70" s="30"/>
-      <c r="W70" s="30"/>
-      <c r="X70" s="30"/>
-      <c r="Y70" s="30"/>
-      <c r="Z70" s="30"/>
-      <c r="AA70" s="30"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="5"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="5"/>
+      <c r="X70" s="5"/>
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5"/>
+      <c r="AA70" s="5"/>
     </row>
     <row r="71" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B71" s="27">
         <v>11</v>
@@ -5044,14 +5051,14 @@
       <c r="D71" s="28"/>
       <c r="E71" s="28"/>
       <c r="F71" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J71" s="16"/>
       <c r="K71" s="30"/>
@@ -5072,57 +5079,65 @@
       <c r="Z71" s="30"/>
       <c r="AA71" s="30"/>
     </row>
-    <row r="72" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="44">
+    <row r="72" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" s="27">
+        <v>11</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="G72" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="H72" s="29"/>
+      <c r="I72" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J72" s="16"/>
+      <c r="K72" s="30"/>
+      <c r="L72" s="30"/>
+      <c r="M72" s="30"/>
+      <c r="N72" s="30"/>
+      <c r="O72" s="30"/>
+      <c r="P72" s="30"/>
+      <c r="Q72" s="30"/>
+      <c r="R72" s="30"/>
+      <c r="S72" s="30"/>
+      <c r="T72" s="30"/>
+      <c r="U72" s="30"/>
+      <c r="V72" s="30"/>
+      <c r="W72" s="30"/>
+      <c r="X72" s="30"/>
+      <c r="Y72" s="30"/>
+      <c r="Z72" s="30"/>
+      <c r="AA72" s="30"/>
+    </row>
+    <row r="73" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="44">
         <v>7</v>
       </c>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="G72" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="H72" s="48"/>
-      <c r="I72" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
-      <c r="O72" s="5"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="5"/>
-      <c r="S72" s="5"/>
-      <c r="T72" s="5"/>
-      <c r="U72" s="5"/>
-      <c r="V72" s="5"/>
-      <c r="W72" s="5"/>
-      <c r="X72" s="5"/>
-      <c r="Y72" s="5"/>
-      <c r="Z72" s="5"/>
-      <c r="AA72" s="5"/>
-    </row>
-    <row r="73" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="44"/>
-      <c r="B73" s="44"/>
       <c r="C73" s="46"/>
       <c r="D73" s="46"/>
       <c r="E73" s="46"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="46"/>
+      <c r="F73" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="G73" s="46" t="s">
+        <v>131</v>
+      </c>
       <c r="H73" s="48"/>
-      <c r="I73" s="44"/>
+      <c r="I73" s="44" t="s">
+        <v>95</v>
+      </c>
       <c r="J73" s="4" t="s">
         <v>64</v>
       </c>
@@ -5144,48 +5159,40 @@
       <c r="Z73" s="5"/>
       <c r="AA73" s="5"/>
     </row>
-    <row r="75" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B75" s="32">
-        <v>6</v>
-      </c>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="G75" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="H75" s="33"/>
-      <c r="I75" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="J75" s="21"/>
-      <c r="K75" s="34"/>
-      <c r="L75" s="34"/>
-      <c r="M75" s="34"/>
-      <c r="N75" s="34"/>
-      <c r="O75" s="34"/>
-      <c r="P75" s="34"/>
-      <c r="Q75" s="34"/>
-      <c r="R75" s="34"/>
-      <c r="S75" s="34"/>
-      <c r="T75" s="34"/>
-      <c r="U75" s="34"/>
-      <c r="V75" s="34"/>
-      <c r="W75" s="34"/>
-      <c r="X75" s="34"/>
-      <c r="Y75" s="34"/>
-      <c r="Z75" s="34"/>
-      <c r="AA75" s="34"/>
+    <row r="74" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="48"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+      <c r="AA74" s="5"/>
     </row>
     <row r="76" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" s="32">
         <v>6</v>
@@ -5194,14 +5201,14 @@
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
       <c r="F76" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G76" s="36" t="s">
         <v>232</v>
       </c>
       <c r="H76" s="33"/>
       <c r="I76" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J76" s="21"/>
       <c r="K76" s="34"/>
@@ -5222,167 +5229,169 @@
       <c r="Z76" s="34"/>
       <c r="AA76" s="34"/>
     </row>
-    <row r="77" spans="1:27" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
+    <row r="77" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B77" s="32">
+        <v>6</v>
+      </c>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="G77" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="H77" s="33"/>
+      <c r="I77" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="J77" s="21"/>
+      <c r="K77" s="34"/>
+      <c r="L77" s="34"/>
+      <c r="M77" s="34"/>
+      <c r="N77" s="34"/>
+      <c r="O77" s="34"/>
+      <c r="P77" s="34"/>
+      <c r="Q77" s="34"/>
+      <c r="R77" s="34"/>
+      <c r="S77" s="34"/>
+      <c r="T77" s="34"/>
+      <c r="U77" s="34"/>
+      <c r="V77" s="34"/>
+      <c r="W77" s="34"/>
+      <c r="X77" s="34"/>
+      <c r="Y77" s="34"/>
+      <c r="Z77" s="34"/>
+      <c r="AA77" s="34"/>
+    </row>
+    <row r="78" spans="1:27" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B78" s="8">
+        <v>7</v>
+      </c>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="8">
-        <v>7</v>
-      </c>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10" t="s">
+      <c r="G78" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G77" s="10" t="s">
+      <c r="H78" s="11"/>
+      <c r="I78" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J78" s="4"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3"/>
+      <c r="AA78" s="3"/>
+    </row>
+    <row r="79" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="H77" s="11"/>
-      <c r="I77" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="J77" s="4"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="3"/>
-      <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
-      <c r="V77" s="3"/>
-      <c r="W77" s="3"/>
-      <c r="X77" s="3"/>
-      <c r="Y77" s="3"/>
-      <c r="Z77" s="3"/>
-      <c r="AA77" s="3"/>
-    </row>
-    <row r="78" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B78" s="32">
+      <c r="G79" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="H79" s="33"/>
+      <c r="I79" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="J79" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K79" s="34"/>
+      <c r="L79" s="34"/>
+      <c r="M79" s="34"/>
+      <c r="N79" s="34"/>
+      <c r="O79" s="34"/>
+      <c r="P79" s="34"/>
+      <c r="Q79" s="34"/>
+      <c r="R79" s="34"/>
+      <c r="S79" s="34"/>
+      <c r="T79" s="34"/>
+      <c r="U79" s="34"/>
+      <c r="V79" s="34"/>
+      <c r="W79" s="34"/>
+      <c r="X79" s="34"/>
+      <c r="Y79" s="34"/>
+      <c r="Z79" s="34"/>
+      <c r="AA79" s="34"/>
+    </row>
+    <row r="80" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="33">
         <v>9.5</v>
       </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="G78" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="H78" s="33"/>
-      <c r="I78" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="J78" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K78" s="34"/>
-      <c r="L78" s="34"/>
-      <c r="M78" s="34"/>
-      <c r="N78" s="34"/>
-      <c r="O78" s="34"/>
-      <c r="P78" s="34"/>
-      <c r="Q78" s="34"/>
-      <c r="R78" s="34"/>
-      <c r="S78" s="34"/>
-      <c r="T78" s="34"/>
-      <c r="U78" s="34"/>
-      <c r="V78" s="34"/>
-      <c r="W78" s="34"/>
-      <c r="X78" s="34"/>
-      <c r="Y78" s="34"/>
-      <c r="Z78" s="34"/>
-      <c r="AA78" s="34"/>
-    </row>
-    <row r="79" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B79" s="33">
-        <v>9.5</v>
-      </c>
-      <c r="C79" s="60"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="60"/>
-      <c r="F79" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="G79" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="H79" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="I79" s="32" t="s">
+      <c r="C80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="60"/>
+      <c r="F80" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="J79" s="61"/>
-    </row>
-    <row r="80" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="32">
-        <v>9.5</v>
-      </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="G80" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="H80" s="33"/>
+      <c r="G80" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="H80" s="33" t="s">
+        <v>233</v>
+      </c>
       <c r="I80" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="J80" s="21"/>
-      <c r="K80" s="34"/>
-      <c r="L80" s="34"/>
-      <c r="M80" s="34"/>
-      <c r="N80" s="34"/>
-      <c r="O80" s="34"/>
-      <c r="P80" s="34"/>
-      <c r="Q80" s="34"/>
-      <c r="R80" s="34"/>
-      <c r="S80" s="34"/>
-      <c r="T80" s="34"/>
-      <c r="U80" s="34"/>
-      <c r="V80" s="34"/>
-      <c r="W80" s="34"/>
-      <c r="X80" s="34"/>
-      <c r="Y80" s="34"/>
-      <c r="Z80" s="34"/>
-      <c r="AA80" s="34"/>
+        <v>224</v>
+      </c>
+      <c r="J80" s="61"/>
     </row>
     <row r="81" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B81" s="32">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="C81" s="36"/>
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
-      <c r="F81" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="G81" s="36" t="s">
-        <v>258</v>
+      <c r="F81" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="H81" s="33"/>
-      <c r="I81" s="32"/>
+      <c r="I81" s="32" t="s">
+        <v>121</v>
+      </c>
       <c r="J81" s="21"/>
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
@@ -5402,49 +5411,49 @@
       <c r="Z81" s="34"/>
       <c r="AA81" s="34"/>
     </row>
-    <row r="82" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="B82" s="44">
-        <v>6</v>
-      </c>
-      <c r="C82" s="48"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="44" t="s">
-        <v>255</v>
-      </c>
-      <c r="G82" s="44"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5"/>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
-      <c r="Y82" s="5"/>
-      <c r="Z82" s="5"/>
-      <c r="AA82" s="5"/>
+    <row r="82" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B82" s="32">
+        <v>7</v>
+      </c>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="G82" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="H82" s="33"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+      <c r="M82" s="34"/>
+      <c r="N82" s="34"/>
+      <c r="O82" s="34"/>
+      <c r="P82" s="34"/>
+      <c r="Q82" s="34"/>
+      <c r="R82" s="34"/>
+      <c r="S82" s="34"/>
+      <c r="T82" s="34"/>
+      <c r="U82" s="34"/>
+      <c r="V82" s="34"/>
+      <c r="W82" s="34"/>
+      <c r="X82" s="34"/>
+      <c r="Y82" s="34"/>
+      <c r="Z82" s="34"/>
+      <c r="AA82" s="34"/>
     </row>
     <row r="83" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B83" s="44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C83" s="48"/>
       <c r="D83" s="46"/>
@@ -5476,22 +5485,20 @@
       <c r="Z83" s="5"/>
       <c r="AA83" s="5"/>
     </row>
-    <row r="84" spans="1:27" ht="29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B84" s="44">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="C84" s="48"/>
       <c r="D84" s="46"/>
       <c r="E84" s="46"/>
       <c r="F84" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="G84" s="56" t="s">
-        <v>256</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="G84" s="44"/>
       <c r="H84" s="48"/>
       <c r="I84" s="44"/>
       <c r="J84" s="4" t="s">
@@ -5515,20 +5522,22 @@
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
     </row>
-    <row r="85" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B85" s="44">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C85" s="48"/>
       <c r="D85" s="46"/>
       <c r="E85" s="46"/>
       <c r="F85" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="G85" s="44"/>
+        <v>147</v>
+      </c>
+      <c r="G85" s="56" t="s">
+        <v>255</v>
+      </c>
       <c r="H85" s="48"/>
       <c r="I85" s="44"/>
       <c r="J85" s="4" t="s">
@@ -5553,14 +5562,20 @@
       <c r="AA85" s="5"/>
     </row>
     <row r="86" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="46"/>
+      <c r="A86" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="44">
+        <v>4.5</v>
+      </c>
+      <c r="C86" s="48"/>
       <c r="D86" s="46"/>
       <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="44"/>
+      <c r="F86" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G86" s="44"/>
+      <c r="H86" s="48"/>
       <c r="I86" s="44"/>
       <c r="J86" s="4" t="s">
         <v>64</v>
@@ -5583,89 +5598,81 @@
       <c r="Z86" s="5"/>
       <c r="AA86" s="5"/>
     </row>
-    <row r="87" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="57"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="30"/>
-      <c r="L87" s="30"/>
-      <c r="M87" s="30"/>
-      <c r="N87" s="30"/>
-      <c r="O87" s="30"/>
-      <c r="P87" s="30"/>
-      <c r="Q87" s="30"/>
-      <c r="R87" s="30"/>
-      <c r="S87" s="30"/>
-      <c r="T87" s="30"/>
-      <c r="U87" s="30"/>
-      <c r="V87" s="30"/>
-      <c r="W87" s="30"/>
-      <c r="X87" s="30"/>
-      <c r="Y87" s="30"/>
-      <c r="Z87" s="30"/>
-      <c r="AA87" s="30"/>
-    </row>
-    <row r="88" spans="1:27" ht="29" x14ac:dyDescent="0.25">
-      <c r="A88" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B88" s="44">
-        <v>5</v>
-      </c>
-      <c r="C88" s="48"/>
-      <c r="D88" s="46"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="G88" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="4" t="s">
+    <row r="87" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="46"/>
+      <c r="D87" s="46"/>
+      <c r="E87" s="46"/>
+      <c r="F87" s="46"/>
+      <c r="G87" s="46"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-      <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
-      <c r="R88" s="5"/>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="5"/>
-      <c r="V88" s="5"/>
-      <c r="W88" s="5"/>
-      <c r="X88" s="5"/>
-      <c r="Y88" s="5"/>
-      <c r="Z88" s="5"/>
-      <c r="AA88" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+      <c r="T87" s="5"/>
+      <c r="U87" s="5"/>
+      <c r="V87" s="5"/>
+      <c r="W87" s="5"/>
+      <c r="X87" s="5"/>
+      <c r="Y87" s="5"/>
+      <c r="Z87" s="5"/>
+      <c r="AA87" s="5"/>
+    </row>
+    <row r="88" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="57"/>
+      <c r="H88" s="27"/>
+      <c r="I88" s="27"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="30"/>
+      <c r="L88" s="30"/>
+      <c r="M88" s="30"/>
+      <c r="N88" s="30"/>
+      <c r="O88" s="30"/>
+      <c r="P88" s="30"/>
+      <c r="Q88" s="30"/>
+      <c r="R88" s="30"/>
+      <c r="S88" s="30"/>
+      <c r="T88" s="30"/>
+      <c r="U88" s="30"/>
+      <c r="V88" s="30"/>
+      <c r="W88" s="30"/>
+      <c r="X88" s="30"/>
+      <c r="Y88" s="30"/>
+      <c r="Z88" s="30"/>
+      <c r="AA88" s="30"/>
     </row>
     <row r="89" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B89" s="44">
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="C89" s="48"/>
       <c r="D89" s="46"/>
       <c r="E89" s="46"/>
       <c r="F89" s="46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G89" s="50" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H89" s="44"/>
       <c r="I89" s="44"/>
@@ -5690,21 +5697,21 @@
       <c r="Z89" s="5"/>
       <c r="AA89" s="5"/>
     </row>
-    <row r="90" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B90" s="44">
-        <v>5.5</v>
+        <v>12.5</v>
       </c>
       <c r="C90" s="48"/>
       <c r="D90" s="46"/>
       <c r="E90" s="46"/>
       <c r="F90" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="G90" s="46" t="s">
-        <v>184</v>
+        <v>140</v>
+      </c>
+      <c r="G90" s="50" t="s">
+        <v>141</v>
       </c>
       <c r="H90" s="44"/>
       <c r="I90" s="44"/>
@@ -5731,19 +5738,19 @@
     </row>
     <row r="91" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B91" s="44">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="C91" s="48"/>
       <c r="D91" s="46"/>
       <c r="E91" s="46"/>
       <c r="F91" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G91" s="46" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="H91" s="44"/>
       <c r="I91" s="44"/>
@@ -5769,16 +5776,26 @@
       <c r="AA91" s="5"/>
     </row>
     <row r="92" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="44"/>
-      <c r="C92" s="46"/>
+      <c r="A92" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="44">
+        <v>8</v>
+      </c>
+      <c r="C92" s="48"/>
       <c r="D92" s="46"/>
       <c r="E92" s="46"/>
-      <c r="F92" s="46"/>
-      <c r="G92" s="46"/>
+      <c r="F92" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="G92" s="46" t="s">
+        <v>143</v>
+      </c>
       <c r="H92" s="44"/>
       <c r="I92" s="44"/>
-      <c r="J92" s="5"/>
+      <c r="J92" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="K92" s="5"/>
       <c r="L92" s="5"/>
       <c r="M92" s="5"/>
@@ -33956,18 +33973,47 @@
       <c r="Z1063" s="5"/>
       <c r="AA1063" s="5"/>
     </row>
+    <row r="1064" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A1064" s="44"/>
+      <c r="B1064" s="44"/>
+      <c r="C1064" s="46"/>
+      <c r="D1064" s="46"/>
+      <c r="E1064" s="46"/>
+      <c r="F1064" s="46"/>
+      <c r="G1064" s="46"/>
+      <c r="H1064" s="44"/>
+      <c r="I1064" s="44"/>
+      <c r="J1064" s="5"/>
+      <c r="K1064" s="5"/>
+      <c r="L1064" s="5"/>
+      <c r="M1064" s="5"/>
+      <c r="N1064" s="5"/>
+      <c r="O1064" s="5"/>
+      <c r="P1064" s="5"/>
+      <c r="Q1064" s="5"/>
+      <c r="R1064" s="5"/>
+      <c r="S1064" s="5"/>
+      <c r="T1064" s="5"/>
+      <c r="U1064" s="5"/>
+      <c r="V1064" s="5"/>
+      <c r="W1064" s="5"/>
+      <c r="X1064" s="5"/>
+      <c r="Y1064" s="5"/>
+      <c r="Z1064" s="5"/>
+      <c r="AA1064" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C73 B80:C1048576">
+  <conditionalFormatting sqref="B1:C74 B81:C1048576">
     <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="0">
       <formula>LEFT(B1,LEN("0"))="0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75:C78">
+  <conditionalFormatting sqref="B76:C79">
     <cfRule type="beginsWith" dxfId="5" priority="4" operator="beginsWith" text="0">
-      <formula>LEFT(B75,LEN("0"))="0"</formula>
+      <formula>LEFT(B76,LEN("0"))="0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J2 J23:J73 J80:J1048576">
+  <conditionalFormatting sqref="J1:J2 J24:J74 J81:J1048576">
     <cfRule type="containsBlanks" dxfId="4" priority="15">
       <formula>LEN(TRIM(J1))=0</formula>
     </cfRule>
@@ -33987,13 +34033,13 @@
       <formula>LEN(TRIM(J12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J75:J78">
+  <conditionalFormatting sqref="J76:J79">
     <cfRule type="containsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(J75))=0</formula>
+      <formula>LEN(TRIM(J76))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B75:C78 B1:C73 B80:C1048576" xr:uid="{B2735817-CCDF-41C4-8B69-E88013140792}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B76:C79 B1:C74 B81:C1048576" xr:uid="{B2735817-CCDF-41C4-8B69-E88013140792}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -34284,15 +34330,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <GalleryStaff xmlns="56a105ef-d554-4e5a-b291-6e5033c93b16">
@@ -34309,6 +34346,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34331,14 +34377,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2B18D4-1C95-487D-95F8-FD7C2B525302}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -34347,4 +34385,12 @@
     <ds:schemaRef ds:uri="8a84207e-cf22-4960-b0fd-3449eb769caa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed spirit spacing, fixed other spacing, added quads, added credits
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://theartsyndicate.sharepoint.com/sites/TheArtSyndicte/Shared Documents/Assets/SRC/Autoscript/TheArtSyndicateMenu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E334C6E-A6B8-403F-A213-C75DD17948CD}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DF53F74-43E6-4710-8A4E-0DC12010ACF6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="270">
   <si>
     <t>Chapter</t>
   </si>
@@ -400,9 +400,6 @@
   </si>
   <si>
     <t>Hoju</t>
-  </si>
-  <si>
-    <t>NSW</t>
   </si>
   <si>
     <t>Amaro</t>
@@ -837,6 +834,21 @@
   </si>
   <si>
     <t>Sauvignon Blanc, Verdejo Grüner Veltliner,</t>
+  </si>
+  <si>
+    <t>Rouse Hill, Sydney</t>
+  </si>
+  <si>
+    <t>Joadja, Southern Highlands</t>
+  </si>
+  <si>
+    <t>Dolans Bay, Sydney</t>
+  </si>
+  <si>
+    <t>Umina Beach, Central Coast</t>
+  </si>
+  <si>
+    <t>Southern Highlands</t>
   </si>
 </sst>
 </file>
@@ -2070,10 +2082,10 @@
   </sheetPr>
   <dimension ref="A1:AA1064"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2155,22 +2167,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>185</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
@@ -2253,20 +2265,20 @@
         <v>2022</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>37</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -2347,20 +2359,20 @@
         <v>2023</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="I6" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>208</v>
-      </c>
       <c r="J6" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
@@ -2394,20 +2406,20 @@
         <v>2021</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="J7" s="17" t="s">
         <v>192</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -2441,22 +2453,22 @@
         <v>2023</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>37</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -2502,7 +2514,7 @@
         <v>41</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>42</v>
@@ -2539,22 +2551,22 @@
         <v>2014</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
@@ -2576,7 +2588,7 @@
     </row>
     <row r="11" spans="1:27" s="35" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" s="32">
         <v>17</v>
@@ -2588,22 +2600,22 @@
         <v>2021</v>
       </c>
       <c r="E11" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="G11" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>217</v>
-      </c>
       <c r="J11" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
@@ -2625,7 +2637,7 @@
     </row>
     <row r="12" spans="1:27" s="31" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="27">
         <v>14</v>
@@ -2637,22 +2649,22 @@
         <v>2023</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F12" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="H12" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="J12" s="15" t="s">
         <v>203</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>204</v>
       </c>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
@@ -2674,7 +2686,7 @@
     </row>
     <row r="13" spans="1:27" s="31" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="27">
         <v>17</v>
@@ -2686,22 +2698,22 @@
         <v>2022</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
@@ -2735,22 +2747,22 @@
         <v>2023</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
@@ -2787,19 +2799,19 @@
         <v>44</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H15" s="33" t="s">
         <v>46</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
@@ -2833,22 +2845,22 @@
         <v>2022</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G16" s="28" t="s">
         <v>48</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I16" s="29" t="s">
         <v>31</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
@@ -2881,20 +2893,20 @@
         <v>2023</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F17" s="63"/>
       <c r="G17" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="H17" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="I17" s="62" t="s">
         <v>243</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="J17" s="22" t="s">
         <v>244</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>245</v>
       </c>
       <c r="K17" s="65"/>
       <c r="L17" s="65"/>
@@ -2928,11 +2940,11 @@
         <v>2021</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>56</v>
@@ -2941,7 +2953,7 @@
         <v>57</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -2975,22 +2987,22 @@
         <v>2017</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>49</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I19" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -3039,7 +3051,7 @@
         <v>54</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
@@ -3073,22 +3085,22 @@
         <v>2022</v>
       </c>
       <c r="E21" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="28" t="s">
-        <v>152</v>
-      </c>
       <c r="G21" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I21" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -3167,10 +3179,10 @@
       <c r="C23" s="27"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>263</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>264</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="29"/>
@@ -3286,13 +3298,13 @@
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
       <c r="E26" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F26" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H26" s="48"/>
       <c r="I26" s="44" t="s">
@@ -3329,7 +3341,7 @@
       <c r="C27" s="46"/>
       <c r="D27" s="46"/>
       <c r="E27" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" s="46" t="s">
         <v>71</v>
@@ -3370,10 +3382,10 @@
       <c r="C28" s="51"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="51" t="s">
         <v>211</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>212</v>
       </c>
       <c r="G28" s="51"/>
       <c r="H28" s="37"/>
@@ -3412,7 +3424,7 @@
         <v>66</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="33"/>
@@ -3524,7 +3536,7 @@
         <v>76</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H32" s="48"/>
       <c r="I32" s="44"/>
@@ -3712,7 +3724,7 @@
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
       <c r="F37" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G37" s="36" t="s">
         <v>83</v>
@@ -3788,7 +3800,7 @@
       <c r="D39" s="36"/>
       <c r="E39" s="36"/>
       <c r="F39" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -3828,7 +3840,7 @@
         <v>86</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H40" s="33"/>
       <c r="I40" s="32"/>
@@ -3864,10 +3876,10 @@
       <c r="D41" s="36"/>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="32"/>
@@ -3901,10 +3913,10 @@
       <c r="D42" s="36"/>
       <c r="E42" s="36"/>
       <c r="F42" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" s="36" t="s">
         <v>227</v>
-      </c>
-      <c r="G42" s="36" t="s">
-        <v>228</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="32"/>
@@ -4013,7 +4025,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H45" s="48"/>
       <c r="I45" s="44" t="s">
@@ -4054,7 +4066,7 @@
         <v>91</v>
       </c>
       <c r="G46" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H46" s="48"/>
       <c r="I46" s="44" t="s">
@@ -4095,7 +4107,7 @@
         <v>91</v>
       </c>
       <c r="G47" s="36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H47" s="33"/>
       <c r="I47" s="32" t="s">
@@ -4140,7 +4152,7 @@
       </c>
       <c r="H48" s="48"/>
       <c r="I48" s="44" t="s">
-        <v>95</v>
+        <v>266</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>64</v>
@@ -4174,14 +4186,14 @@
       <c r="D49" s="28"/>
       <c r="E49" s="28"/>
       <c r="F49" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="27" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>64</v>
@@ -4339,11 +4351,11 @@
         <v>93</v>
       </c>
       <c r="G53" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H53" s="48"/>
       <c r="I53" s="44" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>64</v>
@@ -4380,11 +4392,11 @@
         <v>93</v>
       </c>
       <c r="G54" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H54" s="48"/>
       <c r="I54" s="44" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>64</v>
@@ -4425,7 +4437,7 @@
       </c>
       <c r="H55" s="48"/>
       <c r="I55" s="44" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>64</v>
@@ -4753,7 +4765,7 @@
       </c>
       <c r="H63" s="48"/>
       <c r="I63" s="44" t="s">
-        <v>121</v>
+        <v>267</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>64</v>
@@ -4836,7 +4848,7 @@
     </row>
     <row r="66" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="44">
         <v>12</v>
@@ -4845,10 +4857,10 @@
       <c r="D66" s="46"/>
       <c r="E66" s="46"/>
       <c r="F66" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G66" s="46" t="s">
         <v>123</v>
-      </c>
-      <c r="G66" s="46" t="s">
-        <v>124</v>
       </c>
       <c r="H66" s="48"/>
       <c r="I66" s="44" t="s">
@@ -4877,7 +4889,7 @@
     </row>
     <row r="67" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B67" s="32">
         <v>8</v>
@@ -4886,10 +4898,10 @@
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
       <c r="F67" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="G67" s="33" t="s">
         <v>126</v>
-      </c>
-      <c r="G67" s="33" t="s">
-        <v>127</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="32" t="s">
@@ -4918,7 +4930,7 @@
     </row>
     <row r="68" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B68" s="32">
         <v>9</v>
@@ -4930,11 +4942,11 @@
         <v>93</v>
       </c>
       <c r="G68" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H68" s="33"/>
       <c r="I68" s="32" t="s">
-        <v>95</v>
+        <v>266</v>
       </c>
       <c r="J68" s="21" t="s">
         <v>64</v>
@@ -4959,7 +4971,7 @@
     </row>
     <row r="69" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B69" s="32">
         <v>9</v>
@@ -4968,10 +4980,10 @@
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
       <c r="F69" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G69" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H69" s="33"/>
       <c r="I69" s="32" t="s">
@@ -5000,7 +5012,7 @@
     </row>
     <row r="70" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B70" s="44">
         <v>10</v>
@@ -5009,14 +5021,14 @@
       <c r="D70" s="46"/>
       <c r="E70" s="46"/>
       <c r="F70" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G70" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H70" s="48"/>
       <c r="I70" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="5"/>
@@ -5039,7 +5051,7 @@
     </row>
     <row r="71" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B71" s="27">
         <v>11</v>
@@ -5051,7 +5063,7 @@
         <v>99</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="27" t="s">
@@ -5078,7 +5090,7 @@
     </row>
     <row r="72" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B72" s="27">
         <v>11</v>
@@ -5090,7 +5102,7 @@
         <v>99</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="27" t="s">
@@ -5117,7 +5129,7 @@
     </row>
     <row r="73" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B73" s="44">
         <v>7</v>
@@ -5129,7 +5141,7 @@
         <v>93</v>
       </c>
       <c r="G73" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H73" s="48"/>
       <c r="I73" s="44" t="s">
@@ -5189,7 +5201,7 @@
     </row>
     <row r="76" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B76" s="32">
         <v>6</v>
@@ -5198,14 +5210,14 @@
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
       <c r="F76" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G76" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H76" s="33"/>
       <c r="I76" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J76" s="21"/>
       <c r="K76" s="34"/>
@@ -5228,7 +5240,7 @@
     </row>
     <row r="77" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B77" s="32">
         <v>6</v>
@@ -5237,14 +5249,14 @@
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
       <c r="F77" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G77" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H77" s="33"/>
       <c r="I77" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J77" s="21"/>
       <c r="K77" s="34"/>
@@ -5267,7 +5279,7 @@
     </row>
     <row r="78" spans="1:27" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B78" s="8">
         <v>7</v>
@@ -5276,10 +5288,10 @@
       <c r="D78" s="10"/>
       <c r="E78" s="10"/>
       <c r="F78" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G78" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="G78" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="H78" s="11"/>
       <c r="I78" s="8" t="s">
@@ -5306,7 +5318,7 @@
     </row>
     <row r="79" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B79" s="32">
         <v>9.5</v>
@@ -5315,14 +5327,14 @@
       <c r="D79" s="36"/>
       <c r="E79" s="36"/>
       <c r="F79" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H79" s="33"/>
       <c r="I79" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J79" s="21" t="s">
         <v>64</v>
@@ -5347,7 +5359,7 @@
     </row>
     <row r="80" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B80" s="33">
         <v>9.5</v>
@@ -5356,22 +5368,22 @@
       <c r="D80" s="60"/>
       <c r="E80" s="60"/>
       <c r="F80" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G80" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H80" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I80" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J80" s="61"/>
     </row>
     <row r="81" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B81" s="32">
         <v>9.5</v>
@@ -5380,14 +5392,14 @@
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
       <c r="F81" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H81" s="33"/>
       <c r="I81" s="32" t="s">
-        <v>121</v>
+        <v>268</v>
       </c>
       <c r="J81" s="21"/>
       <c r="K81" s="34"/>
@@ -5410,7 +5422,7 @@
     </row>
     <row r="82" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B82" s="32">
         <v>7</v>
@@ -5419,10 +5431,10 @@
       <c r="D82" s="36"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G82" s="36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H82" s="33"/>
       <c r="I82" s="32"/>
@@ -5447,7 +5459,7 @@
     </row>
     <row r="83" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B83" s="44">
         <v>6</v>
@@ -5456,7 +5468,7 @@
       <c r="D83" s="46"/>
       <c r="E83" s="46"/>
       <c r="F83" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G83" s="44"/>
       <c r="H83" s="48"/>
@@ -5484,7 +5496,7 @@
     </row>
     <row r="84" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B84" s="44">
         <v>4</v>
@@ -5493,9 +5505,11 @@
       <c r="D84" s="46"/>
       <c r="E84" s="46"/>
       <c r="F84" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="G84" s="44"/>
+        <v>251</v>
+      </c>
+      <c r="G84" s="44" t="s">
+        <v>253</v>
+      </c>
       <c r="H84" s="48"/>
       <c r="I84" s="44"/>
       <c r="J84" s="4" t="s">
@@ -5519,9 +5533,9 @@
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
     </row>
-    <row r="85" spans="1:27" ht="29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" s="44">
         <v>5.5</v>
@@ -5530,11 +5544,9 @@
       <c r="D85" s="46"/>
       <c r="E85" s="46"/>
       <c r="F85" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="G85" s="56" t="s">
-        <v>254</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="G85" s="56"/>
       <c r="H85" s="48"/>
       <c r="I85" s="44"/>
       <c r="J85" s="4" t="s">
@@ -5560,7 +5572,7 @@
     </row>
     <row r="86" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B86" s="44">
         <v>4.5</v>
@@ -5569,7 +5581,7 @@
       <c r="D86" s="46"/>
       <c r="E86" s="46"/>
       <c r="F86" s="44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G86" s="44"/>
       <c r="H86" s="48"/>
@@ -5657,7 +5669,7 @@
     </row>
     <row r="89" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" s="44">
         <v>5</v>
@@ -5666,10 +5678,10 @@
       <c r="D89" s="46"/>
       <c r="E89" s="46"/>
       <c r="F89" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G89" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H89" s="44"/>
       <c r="I89" s="44"/>
@@ -5696,7 +5708,7 @@
     </row>
     <row r="90" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B90" s="44">
         <v>12.5</v>
@@ -5705,10 +5717,10 @@
       <c r="D90" s="46"/>
       <c r="E90" s="46"/>
       <c r="F90" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="G90" s="50" t="s">
         <v>140</v>
-      </c>
-      <c r="G90" s="50" t="s">
-        <v>141</v>
       </c>
       <c r="H90" s="44"/>
       <c r="I90" s="44"/>
@@ -5735,7 +5747,7 @@
     </row>
     <row r="91" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B91" s="44">
         <v>5.5</v>
@@ -5744,10 +5756,10 @@
       <c r="D91" s="46"/>
       <c r="E91" s="46"/>
       <c r="F91" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G91" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H91" s="44"/>
       <c r="I91" s="44"/>
@@ -5774,7 +5786,7 @@
     </row>
     <row r="92" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B92" s="44">
         <v>8</v>
@@ -5783,10 +5795,10 @@
       <c r="D92" s="46"/>
       <c r="E92" s="46"/>
       <c r="F92" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="G92" s="46" t="s">
         <v>142</v>
-      </c>
-      <c r="G92" s="46" t="s">
-        <v>143</v>
       </c>
       <c r="H92" s="44"/>
       <c r="I92" s="44"/>
@@ -34039,8 +34051,9 @@
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B76:C79 B1:C74 B81:C1048576" xr:uid="{B2735817-CCDF-41C4-8B69-E88013140792}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -34327,6 +34340,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <GalleryStaff xmlns="56a105ef-d554-4e5a-b291-6e5033c93b16">
@@ -34343,15 +34365,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34374,6 +34387,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2B18D4-1C95-487D-95F8-FD7C2B525302}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -34382,12 +34403,4 @@
     <ds:schemaRef ds:uri="8a84207e-cf22-4960-b0fd-3449eb769caa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated spredsheet to fix a missing comma
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://theartsyndicate.sharepoint.com/sites/TheArtSyndicte/Shared Documents/Assets/SRC/Autoscript/TheArtSyndicateMenu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DF53F74-43E6-4710-8A4E-0DC12010ACF6}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{3AB3E104-751F-482D-9AE7-2B9E179BEC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEC87157-EA23-432E-A84F-0DA2E773A586}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="267">
   <si>
     <t>Chapter</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Riesling</t>
-  </si>
-  <si>
-    <t>Nashdale, Orange region</t>
   </si>
   <si>
     <t>The Little Wine Company</t>
@@ -322,9 +319,6 @@
   </si>
   <si>
     <t>Barrel Aged Gin</t>
-  </si>
-  <si>
-    <t>Joadja</t>
   </si>
   <si>
     <t>Vodka</t>
@@ -592,9 +586,6 @@
     <t>Monica Gray</t>
   </si>
   <si>
-    <t>Nashdale, Orange Region</t>
-  </si>
-  <si>
     <t>"Balance"</t>
   </si>
   <si>
@@ -746,9 +737,6 @@
     <t xml:space="preserve">Chapter Tea </t>
   </si>
   <si>
-    <t>Tumblong Hill's philosophy is all about thoughtful vineyard practices, respecting nature and working to protect the environment. Chenin Blanc is originally from France but has found perfect growing conditions in NSW with classic notes of honeysuckle, pear and quince.</t>
-  </si>
-  <si>
     <t>Sangiovese, Graciano, Merlot, Shiraz, Cabernet Sauvignon</t>
   </si>
   <si>
@@ -800,9 +788,6 @@
     <t xml:space="preserve">Selection of T2 teas </t>
   </si>
   <si>
-    <t>Numero Uno Coffee Roasters, St Peters.</t>
-  </si>
-  <si>
     <t>Yuzu Sake Lemonade</t>
   </si>
   <si>
@@ -839,9 +824,6 @@
     <t>Rouse Hill, Sydney</t>
   </si>
   <si>
-    <t>Joadja, Southern Highlands</t>
-  </si>
-  <si>
     <t>Dolans Bay, Sydney</t>
   </si>
   <si>
@@ -849,6 +831,15 @@
   </si>
   <si>
     <t>Southern Highlands</t>
+  </si>
+  <si>
+    <t>Sourthern Highlands</t>
+  </si>
+  <si>
+    <t>Numero Uno Coffee Roasters, St Peters</t>
+  </si>
+  <si>
+    <t>Tumblong Hills' philosophy is all about thoughtful vineyard practices, respecting nature and working to protect the environment. Chenin Blanc is originally from France but has found perfect growing conditions in NSW with classic notes of honeysuckle, pear and quince.</t>
   </si>
 </sst>
 </file>
@@ -2083,9 +2074,9 @@
   <dimension ref="A1:AA1064"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2167,22 +2158,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
@@ -2265,20 +2256,20 @@
         <v>2022</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -2312,20 +2303,20 @@
         <v>2023</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="J5" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -2359,20 +2350,20 @@
         <v>2023</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="37" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
@@ -2406,20 +2397,20 @@
         <v>2021</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -2453,22 +2444,22 @@
         <v>2023</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -2502,22 +2493,22 @@
         <v>2021</v>
       </c>
       <c r="E9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="G9" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="H9" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="I9" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
@@ -2551,22 +2542,22 @@
         <v>2014</v>
       </c>
       <c r="E10" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
@@ -2588,7 +2579,7 @@
     </row>
     <row r="11" spans="1:27" s="35" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B11" s="32">
         <v>17</v>
@@ -2600,22 +2591,22 @@
         <v>2021</v>
       </c>
       <c r="E11" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>217</v>
-      </c>
       <c r="I11" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
@@ -2637,7 +2628,7 @@
     </row>
     <row r="12" spans="1:27" s="31" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="27">
         <v>14</v>
@@ -2649,22 +2640,22 @@
         <v>2023</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F12" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="I12" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="J12" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>203</v>
       </c>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
@@ -2686,7 +2677,7 @@
     </row>
     <row r="13" spans="1:27" s="31" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B13" s="27">
         <v>17</v>
@@ -2698,22 +2689,22 @@
         <v>2022</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
@@ -2735,7 +2726,7 @@
     </row>
     <row r="14" spans="1:27" s="35" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="32">
         <v>15</v>
@@ -2747,22 +2738,22 @@
         <v>2023</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
@@ -2784,7 +2775,7 @@
     </row>
     <row r="15" spans="1:27" s="35" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="32">
         <v>17</v>
@@ -2796,22 +2787,22 @@
         <v>2023</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
@@ -2833,7 +2824,7 @@
     </row>
     <row r="16" spans="1:27" s="42" customFormat="1" ht="89.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="27">
         <v>18</v>
@@ -2845,22 +2836,22 @@
         <v>2022</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="J16" s="40" t="s">
         <v>194</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="40" t="s">
-        <v>197</v>
       </c>
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
@@ -2881,7 +2872,7 @@
     </row>
     <row r="17" spans="1:27" s="66" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="62">
         <v>14</v>
@@ -2893,20 +2884,20 @@
         <v>2023</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F17" s="63"/>
       <c r="G17" s="62" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H17" s="64" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I17" s="62" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="K17" s="65"/>
       <c r="L17" s="65"/>
@@ -2928,7 +2919,7 @@
     </row>
     <row r="18" spans="1:27" s="31" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="27">
         <v>15</v>
@@ -2940,20 +2931,20 @@
         <v>2021</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="43" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H18" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I18" s="27" t="s">
-        <v>57</v>
-      </c>
       <c r="J18" s="17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -2975,7 +2966,7 @@
     </row>
     <row r="19" spans="1:27" s="31" customFormat="1" ht="101.5" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="27">
         <v>16</v>
@@ -2987,22 +2978,22 @@
         <v>2017</v>
       </c>
       <c r="E19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="I19" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="G19" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -3024,7 +3015,7 @@
     </row>
     <row r="20" spans="1:27" s="31" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="27">
         <v>23</v>
@@ -3036,22 +3027,22 @@
         <v>2010</v>
       </c>
       <c r="E20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="G20" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="H20" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="I20" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="27" t="s">
-        <v>54</v>
-      </c>
       <c r="J20" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
@@ -3073,7 +3064,7 @@
     </row>
     <row r="21" spans="1:27" s="31" customFormat="1" ht="101.5" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="27">
         <v>12</v>
@@ -3085,22 +3076,22 @@
         <v>2022</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -3122,7 +3113,7 @@
     </row>
     <row r="22" spans="1:27" s="31" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="27">
         <v>12</v>
@@ -3134,22 +3125,22 @@
         <v>22</v>
       </c>
       <c r="E22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="G22" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="29" t="s">
+      <c r="I22" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="J22" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
@@ -3171,7 +3162,7 @@
     </row>
     <row r="23" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="27">
         <v>9.5</v>
@@ -3179,10 +3170,10 @@
       <c r="C23" s="27"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="29"/>
@@ -3208,7 +3199,7 @@
     </row>
     <row r="24" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="44">
         <v>13</v>
@@ -3216,18 +3207,18 @@
       <c r="C24" s="46"/>
       <c r="D24" s="46"/>
       <c r="E24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="47" t="s">
         <v>66</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>67</v>
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="48"/>
       <c r="I24" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -3249,7 +3240,7 @@
     </row>
     <row r="25" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="44">
         <v>13</v>
@@ -3257,18 +3248,18 @@
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
       <c r="E25" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="44"/>
       <c r="H25" s="48"/>
       <c r="I25" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -3290,7 +3281,7 @@
     </row>
     <row r="26" spans="1:27" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="44">
         <v>13</v>
@@ -3298,20 +3289,20 @@
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
       <c r="E26" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="46" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H26" s="48"/>
       <c r="I26" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -3333,7 +3324,7 @@
     </row>
     <row r="27" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="44">
         <v>12</v>
@@ -3341,18 +3332,18 @@
       <c r="C27" s="46"/>
       <c r="D27" s="46"/>
       <c r="E27" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="46"/>
       <c r="H27" s="48"/>
       <c r="I27" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -3374,7 +3365,7 @@
     </row>
     <row r="28" spans="1:27" s="53" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="37">
         <v>15</v>
@@ -3382,15 +3373,15 @@
       <c r="C28" s="51"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G28" s="51"/>
       <c r="H28" s="37"/>
       <c r="I28" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J28" s="19"/>
       <c r="K28" s="52"/>
@@ -3413,7 +3404,7 @@
     </row>
     <row r="29" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="32">
         <v>13</v>
@@ -3421,15 +3412,15 @@
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
       <c r="E29" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="33"/>
       <c r="I29" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="34"/>
@@ -3452,7 +3443,7 @@
     </row>
     <row r="30" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="44">
         <v>10</v>
@@ -3460,18 +3451,18 @@
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
       <c r="E30" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="46" t="s">
         <v>72</v>
-      </c>
-      <c r="F30" s="46" t="s">
-        <v>73</v>
       </c>
       <c r="G30" s="46"/>
       <c r="H30" s="48"/>
       <c r="I30" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -3502,7 +3493,7 @@
       <c r="H31" s="48"/>
       <c r="I31" s="44"/>
       <c r="J31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -3524,7 +3515,7 @@
     </row>
     <row r="32" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="44">
         <v>22</v>
@@ -3533,15 +3524,15 @@
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
       <c r="F32" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H32" s="48"/>
       <c r="I32" s="44"/>
       <c r="J32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -3563,7 +3554,7 @@
     </row>
     <row r="33" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="44">
         <v>23</v>
@@ -3572,15 +3563,15 @@
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
       <c r="F33" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="46" t="s">
         <v>77</v>
-      </c>
-      <c r="G33" s="46" t="s">
-        <v>78</v>
       </c>
       <c r="H33" s="48"/>
       <c r="I33" s="44"/>
       <c r="J33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -3602,7 +3593,7 @@
     </row>
     <row r="34" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="44">
         <v>22</v>
@@ -3611,15 +3602,15 @@
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="46" t="s">
         <v>79</v>
-      </c>
-      <c r="G34" s="46" t="s">
-        <v>80</v>
       </c>
       <c r="H34" s="48"/>
       <c r="I34" s="44"/>
       <c r="J34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -3641,7 +3632,7 @@
     </row>
     <row r="35" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="44">
         <v>19</v>
@@ -3650,13 +3641,13 @@
       <c r="D35" s="46"/>
       <c r="E35" s="46"/>
       <c r="F35" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G35" s="46"/>
       <c r="H35" s="48"/>
       <c r="I35" s="44"/>
       <c r="J35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -3678,7 +3669,7 @@
     </row>
     <row r="36" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="44">
         <v>20</v>
@@ -3687,13 +3678,13 @@
       <c r="D36" s="46"/>
       <c r="E36" s="46"/>
       <c r="F36" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G36" s="46"/>
       <c r="H36" s="48"/>
       <c r="I36" s="44"/>
       <c r="J36" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -3715,7 +3706,7 @@
     </row>
     <row r="37" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="32">
         <v>12</v>
@@ -3724,15 +3715,15 @@
       <c r="D37" s="36"/>
       <c r="E37" s="36"/>
       <c r="F37" s="36" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="32"/>
       <c r="J37" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
@@ -3754,7 +3745,7 @@
     </row>
     <row r="38" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="44">
         <v>24</v>
@@ -3763,13 +3754,13 @@
       <c r="D38" s="46"/>
       <c r="E38" s="46"/>
       <c r="F38" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G38" s="46"/>
       <c r="H38" s="48"/>
       <c r="I38" s="44"/>
       <c r="J38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -3791,7 +3782,7 @@
     </row>
     <row r="39" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="32">
         <v>22</v>
@@ -3800,13 +3791,13 @@
       <c r="D39" s="36"/>
       <c r="E39" s="36"/>
       <c r="F39" s="36" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
       <c r="I39" s="32"/>
       <c r="J39" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
@@ -3828,7 +3819,7 @@
     </row>
     <row r="40" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" s="32">
         <v>12</v>
@@ -3837,15 +3828,15 @@
       <c r="D40" s="36"/>
       <c r="E40" s="36"/>
       <c r="F40" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H40" s="33"/>
       <c r="I40" s="32"/>
       <c r="J40" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
@@ -3867,7 +3858,7 @@
     </row>
     <row r="41" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" s="32">
         <v>10</v>
@@ -3876,10 +3867,10 @@
       <c r="D41" s="36"/>
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="32"/>
@@ -3904,7 +3895,7 @@
     </row>
     <row r="42" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="32">
         <v>12</v>
@@ -3913,10 +3904,10 @@
       <c r="D42" s="36"/>
       <c r="E42" s="36"/>
       <c r="F42" s="36" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G42" s="36" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="32"/>
@@ -3950,7 +3941,7 @@
       <c r="H43" s="48"/>
       <c r="I43" s="44"/>
       <c r="J43" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -3972,7 +3963,7 @@
     </row>
     <row r="44" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="32">
         <v>10</v>
@@ -3981,17 +3972,17 @@
       <c r="D44" s="36"/>
       <c r="E44" s="36"/>
       <c r="F44" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="36" t="s">
         <v>88</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>89</v>
       </c>
       <c r="H44" s="33"/>
       <c r="I44" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
@@ -4013,7 +4004,7 @@
     </row>
     <row r="45" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="44">
         <v>13</v>
@@ -4022,17 +4013,17 @@
       <c r="D45" s="46"/>
       <c r="E45" s="46"/>
       <c r="F45" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G45" s="46" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H45" s="48"/>
       <c r="I45" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -4054,7 +4045,7 @@
     </row>
     <row r="46" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="44">
         <v>13</v>
@@ -4063,17 +4054,17 @@
       <c r="D46" s="46"/>
       <c r="E46" s="46"/>
       <c r="F46" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46" s="46" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H46" s="48"/>
       <c r="I46" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -4095,7 +4086,7 @@
     </row>
     <row r="47" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" s="32">
         <v>14</v>
@@ -4104,17 +4095,17 @@
       <c r="D47" s="36"/>
       <c r="E47" s="36"/>
       <c r="F47" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G47" s="36" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H47" s="33"/>
       <c r="I47" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
@@ -4136,7 +4127,7 @@
     </row>
     <row r="48" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="48">
         <v>16</v>
@@ -4145,17 +4136,17 @@
       <c r="D48" s="46"/>
       <c r="E48" s="46"/>
       <c r="F48" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="46" t="s">
         <v>93</v>
-      </c>
-      <c r="G48" s="46" t="s">
-        <v>94</v>
       </c>
       <c r="H48" s="48"/>
       <c r="I48" s="44" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
@@ -4177,7 +4168,7 @@
     </row>
     <row r="49" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="27">
         <v>10</v>
@@ -4186,17 +4177,17 @@
       <c r="D49" s="28"/>
       <c r="E49" s="28"/>
       <c r="F49" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>175</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="27" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
@@ -4218,7 +4209,7 @@
     </row>
     <row r="50" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50" s="44">
         <v>10.5</v>
@@ -4227,17 +4218,17 @@
       <c r="D50" s="46"/>
       <c r="E50" s="46"/>
       <c r="F50" s="55" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G50" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H50" s="48"/>
       <c r="I50" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
@@ -4259,7 +4250,7 @@
     </row>
     <row r="51" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B51" s="44">
         <v>11</v>
@@ -4268,17 +4259,17 @@
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
       <c r="F51" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G51" s="46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H51" s="48"/>
       <c r="I51" s="44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -4300,7 +4291,7 @@
     </row>
     <row r="52" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B52" s="44">
         <v>12</v>
@@ -4309,14 +4300,14 @@
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
       <c r="F52" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G52" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H52" s="48"/>
       <c r="I52" s="44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="5"/>
@@ -4339,7 +4330,7 @@
     </row>
     <row r="53" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B53" s="44">
         <v>20</v>
@@ -4348,17 +4339,17 @@
       <c r="D53" s="46"/>
       <c r="E53" s="46"/>
       <c r="F53" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G53" s="50" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H53" s="48"/>
       <c r="I53" s="44" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
@@ -4380,7 +4371,7 @@
     </row>
     <row r="54" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B54" s="44">
         <v>25</v>
@@ -4389,17 +4380,17 @@
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
       <c r="F54" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G54" s="50" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H54" s="48"/>
       <c r="I54" s="44" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -4421,7 +4412,7 @@
     </row>
     <row r="55" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B55" s="44">
         <v>20</v>
@@ -4430,17 +4421,17 @@
       <c r="D55" s="46"/>
       <c r="E55" s="46"/>
       <c r="F55" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G55" s="50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H55" s="48"/>
       <c r="I55" s="44" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -4462,7 +4453,7 @@
     </row>
     <row r="56" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B56" s="44">
         <v>15</v>
@@ -4471,17 +4462,17 @@
       <c r="D56" s="46"/>
       <c r="E56" s="46"/>
       <c r="F56" s="46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G56" s="46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H56" s="48"/>
       <c r="I56" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -4503,7 +4494,7 @@
     </row>
     <row r="57" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B57" s="44">
         <v>18</v>
@@ -4512,17 +4503,17 @@
       <c r="D57" s="46"/>
       <c r="E57" s="46"/>
       <c r="F57" s="46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G57" s="46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H57" s="48"/>
       <c r="I57" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
@@ -4544,7 +4535,7 @@
     </row>
     <row r="58" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B58" s="44">
         <v>25</v>
@@ -4553,17 +4544,17 @@
       <c r="D58" s="46"/>
       <c r="E58" s="46"/>
       <c r="F58" s="46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G58" s="46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H58" s="48"/>
       <c r="I58" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
@@ -4585,7 +4576,7 @@
     </row>
     <row r="59" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B59" s="44">
         <v>20</v>
@@ -4594,17 +4585,17 @@
       <c r="D59" s="46"/>
       <c r="E59" s="46"/>
       <c r="F59" s="46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G59" s="46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H59" s="48"/>
       <c r="I59" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
@@ -4626,7 +4617,7 @@
     </row>
     <row r="60" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B60" s="44">
         <v>13</v>
@@ -4635,17 +4626,17 @@
       <c r="D60" s="46"/>
       <c r="E60" s="46"/>
       <c r="F60" s="46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G60" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H60" s="48"/>
       <c r="I60" s="44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -4667,7 +4658,7 @@
     </row>
     <row r="61" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B61" s="44">
         <v>12</v>
@@ -4676,17 +4667,17 @@
       <c r="D61" s="46"/>
       <c r="E61" s="46"/>
       <c r="F61" s="46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G61" s="46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H61" s="48"/>
       <c r="I61" s="44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -4708,7 +4699,7 @@
     </row>
     <row r="62" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" s="44">
         <v>13</v>
@@ -4717,17 +4708,17 @@
       <c r="D62" s="46"/>
       <c r="E62" s="46"/>
       <c r="F62" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G62" s="46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H62" s="48"/>
       <c r="I62" s="44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
@@ -4749,7 +4740,7 @@
     </row>
     <row r="63" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B63" s="44">
         <v>13</v>
@@ -4758,17 +4749,17 @@
       <c r="D63" s="46"/>
       <c r="E63" s="46"/>
       <c r="F63" s="46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G63" s="46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H63" s="48"/>
       <c r="I63" s="44" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -4848,7 +4839,7 @@
     </row>
     <row r="66" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B66" s="44">
         <v>12</v>
@@ -4857,17 +4848,17 @@
       <c r="D66" s="46"/>
       <c r="E66" s="46"/>
       <c r="F66" s="46" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G66" s="46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H66" s="48"/>
       <c r="I66" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
@@ -4889,7 +4880,7 @@
     </row>
     <row r="67" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B67" s="32">
         <v>8</v>
@@ -4898,17 +4889,17 @@
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
       <c r="F67" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G67" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H67" s="33"/>
       <c r="I67" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J67" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K67" s="34"/>
       <c r="L67" s="34"/>
@@ -4930,7 +4921,7 @@
     </row>
     <row r="68" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B68" s="32">
         <v>9</v>
@@ -4939,17 +4930,17 @@
       <c r="D68" s="36"/>
       <c r="E68" s="36"/>
       <c r="F68" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G68" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H68" s="33"/>
       <c r="I68" s="32" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J68" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K68" s="34"/>
       <c r="L68" s="34"/>
@@ -4971,7 +4962,7 @@
     </row>
     <row r="69" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69" s="32">
         <v>9</v>
@@ -4980,17 +4971,17 @@
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
       <c r="F69" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G69" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H69" s="33"/>
       <c r="I69" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J69" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K69" s="34"/>
       <c r="L69" s="34"/>
@@ -5012,7 +5003,7 @@
     </row>
     <row r="70" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B70" s="44">
         <v>10</v>
@@ -5021,14 +5012,14 @@
       <c r="D70" s="46"/>
       <c r="E70" s="46"/>
       <c r="F70" s="46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G70" s="46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H70" s="48"/>
       <c r="I70" s="44" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="5"/>
@@ -5051,7 +5042,7 @@
     </row>
     <row r="71" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B71" s="27">
         <v>11</v>
@@ -5060,14 +5051,14 @@
       <c r="D71" s="28"/>
       <c r="E71" s="28"/>
       <c r="F71" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J71" s="16"/>
       <c r="K71" s="30"/>
@@ -5090,7 +5081,7 @@
     </row>
     <row r="72" spans="1:27" s="31" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B72" s="27">
         <v>11</v>
@@ -5099,14 +5090,14 @@
       <c r="D72" s="28"/>
       <c r="E72" s="28"/>
       <c r="F72" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J72" s="16"/>
       <c r="K72" s="30"/>
@@ -5129,7 +5120,7 @@
     </row>
     <row r="73" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B73" s="44">
         <v>7</v>
@@ -5138,17 +5129,17 @@
       <c r="D73" s="46"/>
       <c r="E73" s="46"/>
       <c r="F73" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G73" s="46" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H73" s="48"/>
       <c r="I73" s="44" t="s">
-        <v>95</v>
+        <v>264</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
@@ -5179,7 +5170,7 @@
       <c r="H74" s="48"/>
       <c r="I74" s="44"/>
       <c r="J74" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
@@ -5201,7 +5192,7 @@
     </row>
     <row r="76" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B76" s="32">
         <v>6</v>
@@ -5210,14 +5201,14 @@
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
       <c r="F76" s="36" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G76" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H76" s="33"/>
       <c r="I76" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J76" s="21"/>
       <c r="K76" s="34"/>
@@ -5240,7 +5231,7 @@
     </row>
     <row r="77" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B77" s="32">
         <v>6</v>
@@ -5249,14 +5240,14 @@
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
       <c r="F77" s="36" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G77" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H77" s="33"/>
       <c r="I77" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J77" s="21"/>
       <c r="K77" s="34"/>
@@ -5279,7 +5270,7 @@
     </row>
     <row r="78" spans="1:27" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B78" s="8">
         <v>7</v>
@@ -5288,14 +5279,14 @@
       <c r="D78" s="10"/>
       <c r="E78" s="10"/>
       <c r="F78" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H78" s="11"/>
       <c r="I78" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J78" s="4"/>
       <c r="K78" s="3"/>
@@ -5318,7 +5309,7 @@
     </row>
     <row r="79" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B79" s="32">
         <v>9.5</v>
@@ -5327,17 +5318,17 @@
       <c r="D79" s="36"/>
       <c r="E79" s="36"/>
       <c r="F79" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H79" s="33"/>
       <c r="I79" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J79" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K79" s="34"/>
       <c r="L79" s="34"/>
@@ -5359,7 +5350,7 @@
     </row>
     <row r="80" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B80" s="33">
         <v>9.5</v>
@@ -5368,22 +5359,22 @@
       <c r="D80" s="60"/>
       <c r="E80" s="60"/>
       <c r="F80" s="36" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G80" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="H80" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="H80" s="33" t="s">
-        <v>231</v>
-      </c>
       <c r="I80" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J80" s="61"/>
     </row>
     <row r="81" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B81" s="32">
         <v>9.5</v>
@@ -5392,14 +5383,14 @@
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
       <c r="F81" s="32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H81" s="33"/>
       <c r="I81" s="32" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="J81" s="21"/>
       <c r="K81" s="34"/>
@@ -5422,7 +5413,7 @@
     </row>
     <row r="82" spans="1:27" s="35" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B82" s="32">
         <v>7</v>
@@ -5431,10 +5422,10 @@
       <c r="D82" s="36"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G82" s="36" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H82" s="33"/>
       <c r="I82" s="32"/>
@@ -5459,7 +5450,7 @@
     </row>
     <row r="83" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B83" s="44">
         <v>6</v>
@@ -5468,13 +5459,13 @@
       <c r="D83" s="46"/>
       <c r="E83" s="46"/>
       <c r="F83" s="44" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G83" s="44"/>
       <c r="H83" s="48"/>
       <c r="I83" s="44"/>
       <c r="J83" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
@@ -5496,7 +5487,7 @@
     </row>
     <row r="84" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B84" s="44">
         <v>4</v>
@@ -5505,15 +5496,15 @@
       <c r="D84" s="46"/>
       <c r="E84" s="46"/>
       <c r="F84" s="44" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G84" s="44" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="H84" s="48"/>
       <c r="I84" s="44"/>
       <c r="J84" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
@@ -5535,7 +5526,7 @@
     </row>
     <row r="85" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B85" s="44">
         <v>5.5</v>
@@ -5544,13 +5535,13 @@
       <c r="D85" s="46"/>
       <c r="E85" s="46"/>
       <c r="F85" s="44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G85" s="56"/>
       <c r="H85" s="48"/>
       <c r="I85" s="44"/>
       <c r="J85" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
@@ -5572,7 +5563,7 @@
     </row>
     <row r="86" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B86" s="44">
         <v>4.5</v>
@@ -5581,13 +5572,13 @@
       <c r="D86" s="46"/>
       <c r="E86" s="46"/>
       <c r="F86" s="44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G86" s="44"/>
       <c r="H86" s="48"/>
       <c r="I86" s="44"/>
       <c r="J86" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
@@ -5618,7 +5609,7 @@
       <c r="H87" s="44"/>
       <c r="I87" s="44"/>
       <c r="J87" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
@@ -5669,7 +5660,7 @@
     </row>
     <row r="89" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B89" s="44">
         <v>5</v>
@@ -5678,15 +5669,15 @@
       <c r="D89" s="46"/>
       <c r="E89" s="46"/>
       <c r="F89" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G89" s="50" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H89" s="44"/>
       <c r="I89" s="44"/>
       <c r="J89" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
@@ -5708,7 +5699,7 @@
     </row>
     <row r="90" spans="1:27" ht="29" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B90" s="44">
         <v>12.5</v>
@@ -5717,15 +5708,15 @@
       <c r="D90" s="46"/>
       <c r="E90" s="46"/>
       <c r="F90" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G90" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H90" s="44"/>
       <c r="I90" s="44"/>
       <c r="J90" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
@@ -5747,7 +5738,7 @@
     </row>
     <row r="91" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B91" s="44">
         <v>5.5</v>
@@ -5756,15 +5747,15 @@
       <c r="D91" s="46"/>
       <c r="E91" s="46"/>
       <c r="F91" s="46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G91" s="46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H91" s="44"/>
       <c r="I91" s="44"/>
       <c r="J91" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K91" s="5"/>
       <c r="L91" s="5"/>
@@ -5786,7 +5777,7 @@
     </row>
     <row r="92" spans="1:27" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B92" s="44">
         <v>8</v>
@@ -5795,15 +5786,15 @@
       <c r="D92" s="46"/>
       <c r="E92" s="46"/>
       <c r="F92" s="46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G92" s="46" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H92" s="44"/>
       <c r="I92" s="44"/>
       <c r="J92" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K92" s="5"/>
       <c r="L92" s="5"/>
@@ -34059,6 +34050,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002FFBF14A924A434888B8C157730B70E4" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284b427be1b4793f2c3340e5e67ad08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56a105ef-d554-4e5a-b291-6e5033c93b16" xmlns:ns3="8a84207e-cf22-4960-b0fd-3449eb769caa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="008efe2dc965106f2e3e5232e53409cc" ns2:_="" ns3:_="">
     <xsd:import namespace="56a105ef-d554-4e5a-b291-6e5033c93b16"/>
@@ -34339,15 +34339,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -34368,6 +34359,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79747025-BDB8-4215-B87B-EB47E9578779}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34386,14 +34385,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9874B3-7226-4313-8925-6CE9DA4A9860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2B18D4-1C95-487D-95F8-FD7C2B525302}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
identified beer line issue
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://theartsyndicate.sharepoint.com/sites/TheArtSyndicte/Shared Documents/Assets/SRC/Autoscript/TheArtSyndicateMenu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6600DDEA7A9D30A3CAEF30D588CDE6E726B1BD28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89DD2278-5F7A-42C8-9E2E-E9DFE209F73A}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_6600DDEA7A9D30A3CAEF30D588CDE6E726B1BD28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2B21470-77A2-46AF-93C9-BCAB304A4490}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="1440" windowWidth="29040" windowHeight="12510" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>Nashdale, Orange Region</t>
   </si>
   <si>
-    <t xml:space="preserve">With over 30 years experience, the family run business is becoming one of Australia's leading organic wine labels. This fresh wine screams lemon sherbet and freshly cut green apple. </t>
-  </si>
-  <si>
     <t> </t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Jeir, Canberra District</t>
   </si>
   <si>
-    <t>Making wine since the 1970s, Greg’s Blanc de Blanc is a great example of his meticulous approach to winemaking. Made in the “traditional method”, this current vintage was aged for 7 years and developed beautiful aromas of honeydew melon, buttery pastry and a creamy texture.</t>
-  </si>
-  <si>
     <t>Topper's Mountain Wines</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
   </si>
   <si>
     <t>New England</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High up above 900m, the ten hectare vineyard specialises in alternative varieties. The Kirkby's don't use any pesticides, but rather promote a balanced ecosystem that is able to help itself. As the only sparkling Nebbiolo made in Australia, it is full of fresh rosehip and wild strawberry aromas with a creamy texture. </t>
   </si>
   <si>
     <t>Wine - White</t>
@@ -183,9 +174,6 @@
     <t>Orange, Mudgee</t>
   </si>
   <si>
-    <t xml:space="preserve">Taking inspiration from her travels and great wines from around the world, Sam focuses on crafting small-batch, single-vineyard wines, to be enjoyed and shared in good company. The wine is full of zesty citrus notes, while gentle oak ageing gives a pleasant texture. </t>
-  </si>
-  <si>
     <t>Mada Wines</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t>Hilltops</t>
   </si>
   <si>
-    <t xml:space="preserve">Dedicated to showcasing the potential of the Canberra, Hilltops, and Tumbarumba regions, Hamish collaborates with viticulturalists who share his philosophy. This is a generous blend, with aromas of orange blossom, fresh lychee and lots of zestiness. </t>
-  </si>
-  <si>
     <t>Tumblong Hills</t>
   </si>
   <si>
@@ -214,9 +199,6 @@
   </si>
   <si>
     <t>Gundagai</t>
-  </si>
-  <si>
-    <t>Tumblong Hills' philosophy is all about thoughtful vineyard practices, respecting nature and working to protect the environment. Chenin Blanc is originally from France but has found perfect growing conditions in NSW with classic notes of honeysuckle, pear and quince.</t>
   </si>
   <si>
     <t>Wondalma Vineyard</t>
@@ -241,9 +223,6 @@
   </si>
   <si>
     <t>Orange</t>
-  </si>
-  <si>
-    <t>Meeting in the Master of Wine program, the winemakers connected over their passion for small-batch, terroir driven wine. The thoughtful approach to winemaking and long oak maturation created a layered, ever evolving wine with aromas of lemon curd, fresh yellow apple and baking spices.</t>
   </si>
   <si>
     <t>Matthew Attalah Wines</t>
@@ -276,9 +255,6 @@
     <t>Pokolbin, Hunter Valley</t>
   </si>
   <si>
-    <t>Being named Halliday Winemaker of the Year 2025, Liz’s vision is to make some of the best small batch contemporary versions of traditional Hunter varieties. This aged Semillon shows intense flavours of preserved lemon, chamomile and mouthcoating notes of crème brulee and green almonds.</t>
-  </si>
-  <si>
     <t>Wine - Amber</t>
   </si>
   <si>
@@ -286,9 +262,6 @@
   </si>
   <si>
     <t>Sauvignon Blanc, Verdejo, Grüner Veltliner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High up above 900m, the ten hectare vineyard specialises in alternative varieties. The Hill of Dreams is a place of diversity and experimentation. The different varieties are spontaneously fermented on their skins for texture and fragrant notes of jalapeno, preserved lemon and gooseberry compote.  </t>
   </si>
   <si>
     <t>Wine - Rosé</t>
@@ -348,9 +321,6 @@
     <t>O'Connell Valley, Central Ranges</t>
   </si>
   <si>
-    <t>The Renzaglia family sees themselves as `Stewards of the vines' with a balanced ecosystem in mind. Their "di Renzo" label explores unique styles through innovative and creative winemaking techniques. This chilled red is full of fresh, crunchy fruit and savoury herbaceousness.</t>
-  </si>
-  <si>
     <t>Sabi Wabi</t>
   </si>
   <si>
@@ -366,9 +336,6 @@
     <t>Hunter Valley</t>
   </si>
   <si>
-    <t xml:space="preserve">Peta, a Young Gun Of Wine 2022 - Winemaker's Choice winner, is producing small batch, low-intervention wines. The "Nomu" was made entirely in stainless steel, preserving the fresh fruit flavours and delicate aromas in this lighter style. </t>
-  </si>
-  <si>
     <t>Rowlee Wines</t>
   </si>
   <si>
@@ -379,10 +346,6 @@
   </si>
   <si>
     <t>Nicole Samodol and James Manny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handpicking from an eight-hectare vineyard situated on Orange's ancient volcanic soils, the team at Rowlee focus on small batch winemaking with sustainable practices. Layers of crunchy red fruit with notes of cinnamon and liquorice add to the complexity and depth of the wine.
-</t>
   </si>
   <si>
     <t>Whitton Farm</t>
@@ -400,9 +363,6 @@
     <t>Hilltops, Canberra</t>
   </si>
   <si>
-    <t xml:space="preserve">Whitton Farm, driven by a passion for fine Italian wines, produces small-batch handcrafted wines from New South Wales' premium, often overlooked wine regions that share a similar climate to central Italy. The Rosso is a medium bodied blend, boasting red cherries and soft spices. </t>
-  </si>
-  <si>
     <t>The Little Wine Company</t>
   </si>
   <si>
@@ -415,9 +375,6 @@
     <t>Broke, Hunter Valley</t>
   </si>
   <si>
-    <t xml:space="preserve">Suzanne and Ian, both from winemaking backgrounds, joined forces in 2000. Originally from Italy’s northern Piedmont region, this Barbera enjoys the Hunter's long sunshine hours and displays plush red and black berries, and soft tannins. </t>
-  </si>
-  <si>
     <t>Glenguin</t>
   </si>
   <si>
@@ -425,9 +382,6 @@
   </si>
   <si>
     <t>Robin, Rita and Andrew Tedder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Under the guidance of Master of Wine Robin Tedder, the estate follows organic and biodynamic principles to produce limited, high-quality Shiraz and Semillon from vines descended from James Busby’s original 1820s plantings. Powerful yet refined, the wine has notes of ripe berries, dark chocolate and Christmas cake. </t>
   </si>
   <si>
     <t>Quilty Wines</t>
@@ -485,9 +439,6 @@
   </si>
   <si>
     <t>Tap</t>
-  </si>
-  <si>
-    <t>Ask about our latest tap beers, \\ or just look at our tap.</t>
   </si>
   <si>
     <t>Willie the Boatman</t>
@@ -802,9 +753,6 @@
     <t>South Pacific Seltzer</t>
   </si>
   <si>
-    <t>Ginger, Cinnamon, Citrus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chapter Tea </t>
   </si>
   <si>
@@ -863,6 +811,58 @@
   </si>
   <si>
     <t>Broke Fordwich, Hunter Valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With over 30 years experience, this family run business is becoming one of Australia's leading organic wine labels. This fresh wine screams lemon sherbet and freshly cut green apple. </t>
+  </si>
+  <si>
+    <t>Tumblong Hills' philosophy is all about thoughtful vineyard practices, respecting nature and working to protect the environment. Chenin Blanc is originally from France but has found perfect growing conditions in NSW, producing classic notes of honeysuckle, pear and quince.</t>
+  </si>
+  <si>
+    <t>The Renzaglia family sees themselves as "Stewards of the vines" with a balanced ecosystem in mind. Their "di Renzo" label explores unique styles through innovative and creative winemaking techniques. This chilled red is full of fresh, crunchy fruit and savoury herbaceousness.</t>
+  </si>
+  <si>
+    <t>Making wine since the 1970s, Greg's Blanc de Blanc is a great example of his meticulous approach to winemaking. Made in the "traditional method" this current vintage was aged for 7 years and developed beautiful aromas of honeydew melon, buttery pastry and a creamy texture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dedicated to showcasing the potential of the Canberra, Hilltops and Tumbarumba regions, Hamish collaborates with viticulturalists who share his philosophy. This is a generous blend with lots of zestiness and aromas of orange blossom and fresh lychee. </t>
+  </si>
+  <si>
+    <t>Being named Halliday Winemaker of the Year 2025, Liz's vision is to make some of the best small batch contemporary versions of traditional Hunter varieties. This aged Semillon shows intense flavours of preserved lemon, chamomile and mouthcoating notes of crème brulee and green almonds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ten hectare vineyard is located 900m above sea level and specialises in alternative varieties. The Hill of Dreams is a place of diversity and experimentation. The different varieties are spontaneously fermented on their skins for texture and fragrant notes of jalapeno, preserved lemon and gooseberry compote.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High up above 900m, the ten hectare vineyard specialises in alternative varieties. The Kirkbys don't use any pesticides, but rather promote a balanced ecosystem that is able to help itself. As the only sparkling Nebbiolo made in Australia, it is full of fresh rosehip and wild strawberry aromas, with a creamy texture. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handpicking from an eight hectare vineyard situated on Orange's ancient volcanic soils, the team at Rowlee focus on small batch winemaking with sustainable practices. Layers of crunchy red fruit with notes of cinnamon and liquorice add to the complexity and depth of the wine.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taking inspiration from her travels and great wines from around the world, Sam focuses on crafting small batch, single-vineyard wines, to be enjoyed and shared in good company. The wine is full of zesty citrus notes, while gentle oak ageing gives a pleasant texture. </t>
+  </si>
+  <si>
+    <t>Meeting in the Master of Wine program, the winemakers connected over their passion for small batch, terroir driven wine. The thoughtful approach to winemaking and long oak maturation created a layered, ever evolving wine with aromas of lemon curd, fresh yellow apple and baking spices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whitton Farm, driven by a passion for fine Italian wines, produces small batch handcrafted wines from New South Wales' premium, often overlooked wine regions that share a similar climate to central Italy. The Rosso is a medium bodied blend, boasting red cherries and soft spices. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanne and Ian, both from winemaking backgrounds, joined forces in 2000. Originally from Italy's northern Piedmont region, this Barbera enjoys the Hunter's long sunshine hours and displays plush red and black berries, and soft tannins. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under the guidance of Master of Wine Robin Tedder, the estate follows organic and biodynamic principles to produce limited, high-quality Shiraz and Semillon from vines descended from James Busby's original 1820's plantings. Powerful yet refined, the wine has notes of ripe berries, dark chocolate and Christmas cake. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peta,  a "Young Gun Of Wine 2022 - Winemaker's Choice" winner,  is producing small batch, low-intervention wines. The "Nomu" was made entirely in stainless steel,  preserving the fresh fruit flavours and delicate aromas of this lighter style. </t>
+  </si>
+  <si>
+    <t>Ginger, Cinnamon,  Citrus</t>
+  </si>
+  <si>
+    <t>Ask about our latest tap beers,\\  or just look at our tap</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1206,6 +1206,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1683,9 +1686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -1789,58 +1792,58 @@
         <v>28</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="17" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
@@ -1861,22 +1864,22 @@
         <v>2016</v>
       </c>
       <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="K3" s="15" t="s">
-        <v>36</v>
+        <v>261</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
@@ -1914,22 +1917,22 @@
         <v>2021</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="I4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="K4" s="20" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
@@ -1951,7 +1954,7 @@
     </row>
     <row r="5" spans="1:28" s="17" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="18">
         <v>16</v>
@@ -1967,20 +1970,20 @@
         <v>2024</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>48</v>
+        <v>267</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
@@ -2002,7 +2005,7 @@
     </row>
     <row r="6" spans="1:28" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="18">
         <v>15</v>
@@ -2018,22 +2021,22 @@
         <v>2024</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>54</v>
+      <c r="K6" s="61" t="s">
+        <v>262</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
@@ -2055,7 +2058,7 @@
     </row>
     <row r="7" spans="1:28" s="12" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="13">
         <v>14</v>
@@ -2071,20 +2074,20 @@
         <v>2023</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="26" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>59</v>
+        <v>259</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
@@ -2106,7 +2109,7 @@
     </row>
     <row r="8" spans="1:28" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="13">
         <v>18</v>
@@ -2122,20 +2125,20 @@
         <v>2021</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
@@ -2157,7 +2160,7 @@
     </row>
     <row r="9" spans="1:28" s="17" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="13">
         <v>25</v>
@@ -2173,22 +2176,22 @@
         <v>2023</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
@@ -2210,7 +2213,7 @@
     </row>
     <row r="10" spans="1:28" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="18">
         <v>18</v>
@@ -2226,22 +2229,22 @@
         <v>2024</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
@@ -2263,7 +2266,7 @@
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="13">
         <v>27</v>
@@ -2279,22 +2282,22 @@
         <v>2014</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
@@ -2316,7 +2319,7 @@
     </row>
     <row r="12" spans="1:28" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B12" s="13">
         <v>17</v>
@@ -2332,22 +2335,22 @@
         <v>2021</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>83</v>
+        <v>264</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -2369,7 +2372,7 @@
     </row>
     <row r="13" spans="1:28" s="12" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B13" s="13">
         <v>14</v>
@@ -2385,22 +2388,22 @@
         <v>2023</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="14" spans="1:28" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B14" s="13">
         <v>17</v>
@@ -2438,22 +2441,22 @@
         <v>2022</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -2475,7 +2478,7 @@
     </row>
     <row r="15" spans="1:28" s="12" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B15" s="13">
         <v>15</v>
@@ -2491,22 +2494,22 @@
         <v>2023</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>103</v>
+        <v>260</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -2528,7 +2531,7 @@
     </row>
     <row r="16" spans="1:28" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B16" s="13">
         <v>17</v>
@@ -2544,22 +2547,22 @@
         <v>2023</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K16" s="27" t="s">
-        <v>109</v>
+        <v>272</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -2581,7 +2584,7 @@
     </row>
     <row r="17" spans="1:28" s="35" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B17" s="13">
         <v>18</v>
@@ -2597,22 +2600,22 @@
         <v>2022</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>114</v>
+        <v>266</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
@@ -2634,7 +2637,7 @@
     </row>
     <row r="18" spans="1:28" s="17" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B18" s="18">
         <v>14</v>
@@ -2650,22 +2653,22 @@
         <v>2022</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>120</v>
+        <v>269</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
@@ -2687,7 +2690,7 @@
     </row>
     <row r="19" spans="1:28" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B19" s="18">
         <v>15</v>
@@ -2703,20 +2706,20 @@
         <v>2019</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="36" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>125</v>
+        <v>270</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -2736,9 +2739,9 @@
       <c r="AA19" s="21"/>
       <c r="AB19" s="21"/>
     </row>
-    <row r="20" spans="1:28" s="17" customFormat="1" ht="87" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="17" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B20" s="18">
         <v>18</v>
@@ -2754,22 +2757,22 @@
         <v>2018</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2791,7 +2794,7 @@
     </row>
     <row r="21" spans="1:28" s="38" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B21" s="18">
         <v>14</v>
@@ -2807,22 +2810,22 @@
         <v>2015</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
@@ -2844,12 +2847,15 @@
     </row>
     <row r="22" spans="1:28" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B22" s="39">
         <v>8</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10">
+        <f>(Table_1[[#This Row],[Column3]]*3.75)</f>
+        <v>30</v>
+      </c>
       <c r="D22" s="39">
         <v>60</v>
       </c>
@@ -2857,22 +2863,22 @@
         <v>2022</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G22" s="39" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I22" s="39" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="K22" s="41" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
@@ -2894,7 +2900,7 @@
     </row>
     <row r="23" spans="1:28" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B23" s="13">
         <v>12</v>
@@ -2907,22 +2913,22 @@
         <v>23</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
@@ -2944,7 +2950,7 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B24" s="13">
         <v>9.5</v>
@@ -2953,10 +2959,10 @@
       <c r="D24" s="13"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>149</v>
+        <v>274</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="10"/>
@@ -2982,7 +2988,7 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B25" s="42">
         <v>13</v>
@@ -2991,18 +2997,18 @@
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="44" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="H25" s="42"/>
       <c r="I25" s="45"/>
       <c r="J25" s="42" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="K25" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L25" s="46"/>
       <c r="M25" s="46"/>
@@ -3024,7 +3030,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B26" s="42">
         <v>13</v>
@@ -3033,18 +3039,18 @@
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="44" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="H26" s="42"/>
       <c r="I26" s="45"/>
       <c r="J26" s="42" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="K26" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L26" s="46"/>
       <c r="M26" s="46"/>
@@ -3066,7 +3072,7 @@
     </row>
     <row r="27" spans="1:28" ht="29" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B27" s="42">
         <v>13</v>
@@ -3075,20 +3081,20 @@
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="44" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="H27" s="47" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="I27" s="45"/>
       <c r="J27" s="42" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="K27" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L27" s="46"/>
       <c r="M27" s="46"/>
@@ -3110,7 +3116,7 @@
     </row>
     <row r="28" spans="1:28" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B28" s="42">
         <v>12</v>
@@ -3119,18 +3125,18 @@
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="44" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="G28" s="43" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="H28" s="43"/>
       <c r="I28" s="45"/>
       <c r="J28" s="42" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="K28" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L28" s="46"/>
       <c r="M28" s="46"/>
@@ -3152,7 +3158,7 @@
     </row>
     <row r="29" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B29" s="26">
         <v>15</v>
@@ -3161,15 +3167,15 @@
       <c r="D29" s="49"/>
       <c r="E29" s="49"/>
       <c r="F29" s="49" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="H29" s="49"/>
       <c r="I29" s="26"/>
       <c r="J29" s="26" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="K29" s="50"/>
       <c r="L29" s="50"/>
@@ -3192,7 +3198,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B30" s="13">
         <v>13</v>
@@ -3201,15 +3207,15 @@
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
       <c r="F30" s="14" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="H30" s="25"/>
       <c r="I30" s="10"/>
       <c r="J30" s="13" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
@@ -3232,7 +3238,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B31" s="42">
         <v>10</v>
@@ -3241,18 +3247,18 @@
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="43" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="G31" s="43" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H31" s="43"/>
       <c r="I31" s="45"/>
       <c r="J31" s="42" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K31" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L31" s="46"/>
       <c r="M31" s="46"/>
@@ -3284,7 +3290,7 @@
       <c r="I32" s="45"/>
       <c r="J32" s="42"/>
       <c r="K32" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L32" s="46"/>
       <c r="M32" s="46"/>
@@ -3306,7 +3312,7 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B33" s="42">
         <v>22</v>
@@ -3316,15 +3322,15 @@
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
       <c r="G33" s="42" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="I33" s="45"/>
       <c r="J33" s="42"/>
       <c r="K33" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L33" s="46"/>
       <c r="M33" s="46"/>
@@ -3346,7 +3352,7 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B34" s="42">
         <v>23</v>
@@ -3356,15 +3362,15 @@
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
       <c r="G34" s="43" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="H34" s="43" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="I34" s="45"/>
       <c r="J34" s="42"/>
       <c r="K34" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L34" s="46"/>
       <c r="M34" s="46"/>
@@ -3386,7 +3392,7 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B35" s="42">
         <v>22</v>
@@ -3396,15 +3402,15 @@
       <c r="E35" s="43"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="H35" s="43" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="I35" s="45"/>
       <c r="J35" s="42"/>
       <c r="K35" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L35" s="46"/>
       <c r="M35" s="46"/>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B36" s="42">
         <v>19</v>
@@ -3436,13 +3442,13 @@
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
       <c r="G36" s="43" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H36" s="43"/>
       <c r="I36" s="45"/>
       <c r="J36" s="42"/>
       <c r="K36" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L36" s="46"/>
       <c r="M36" s="46"/>
@@ -3464,7 +3470,7 @@
     </row>
     <row r="37" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B37" s="42">
         <v>20</v>
@@ -3474,13 +3480,13 @@
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
       <c r="G37" s="43" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="H37" s="43"/>
       <c r="I37" s="45"/>
       <c r="J37" s="42"/>
       <c r="K37" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
@@ -3502,7 +3508,7 @@
     </row>
     <row r="38" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B38" s="13">
         <v>12</v>
@@ -3512,15 +3518,15 @@
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="H38" s="25" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="13"/>
       <c r="K38" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
@@ -3542,7 +3548,7 @@
     </row>
     <row r="39" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B39" s="13">
         <v>24</v>
@@ -3552,13 +3558,13 @@
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
       <c r="G39" s="25" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="10"/>
       <c r="J39" s="13"/>
       <c r="K39" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
@@ -3580,7 +3586,7 @@
     </row>
     <row r="40" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B40" s="13">
         <v>22</v>
@@ -3590,13 +3596,13 @@
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
       <c r="G40" s="25" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="10"/>
       <c r="J40" s="13"/>
       <c r="K40" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
@@ -3618,7 +3624,7 @@
     </row>
     <row r="41" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B41" s="13">
         <v>12</v>
@@ -3628,15 +3634,15 @@
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
       <c r="G41" s="25" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="H41" s="25" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="13"/>
       <c r="K41" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
@@ -3658,7 +3664,7 @@
     </row>
     <row r="42" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B42" s="13">
         <v>10</v>
@@ -3668,10 +3674,10 @@
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="H42" s="25" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="13"/>
@@ -3696,7 +3702,7 @@
     </row>
     <row r="43" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B43" s="13">
         <v>12</v>
@@ -3706,10 +3712,10 @@
       <c r="E43" s="25"/>
       <c r="F43" s="25"/>
       <c r="G43" s="25" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="H43" s="25" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="13"/>
@@ -3744,7 +3750,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="13"/>
       <c r="K44" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
@@ -3766,7 +3772,7 @@
     </row>
     <row r="45" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B45" s="13">
         <v>10</v>
@@ -3776,17 +3782,17 @@
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="13" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="K45" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
@@ -3808,7 +3814,7 @@
     </row>
     <row r="46" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B46" s="13">
         <v>13</v>
@@ -3818,17 +3824,17 @@
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
       <c r="G46" s="25" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="13" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
@@ -3850,7 +3856,7 @@
     </row>
     <row r="47" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B47" s="13">
         <v>13</v>
@@ -3860,17 +3866,17 @@
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="13" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
@@ -3892,7 +3898,7 @@
     </row>
     <row r="48" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B48" s="13">
         <v>14</v>
@@ -3902,17 +3908,17 @@
       <c r="E48" s="25"/>
       <c r="F48" s="25"/>
       <c r="G48" s="25" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="I48" s="10"/>
       <c r="J48" s="13" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
@@ -3934,7 +3940,7 @@
     </row>
     <row r="49" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B49" s="10">
         <v>16</v>
@@ -3944,17 +3950,17 @@
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="25" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H49" s="25" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="I49" s="10"/>
       <c r="J49" s="13" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K49" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
@@ -3976,7 +3982,7 @@
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B50" s="13">
         <v>10</v>
@@ -3986,17 +3992,17 @@
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="25" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="13" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="K50" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
@@ -4018,7 +4024,7 @@
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B51" s="42">
         <v>10.5</v>
@@ -4028,17 +4034,17 @@
       <c r="E51" s="43"/>
       <c r="F51" s="43"/>
       <c r="G51" s="52" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="H51" s="43" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="I51" s="45"/>
       <c r="J51" s="42" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K51" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L51" s="46"/>
       <c r="M51" s="46"/>
@@ -4060,7 +4066,7 @@
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" s="42" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B52" s="42">
         <v>11</v>
@@ -4070,17 +4076,17 @@
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
       <c r="G52" s="43" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H52" s="43" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="I52" s="45"/>
       <c r="J52" s="42" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="K52" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L52" s="46"/>
       <c r="M52" s="46"/>
@@ -4102,7 +4108,7 @@
     </row>
     <row r="53" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B53" s="42">
         <v>12</v>
@@ -4112,14 +4118,14 @@
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
       <c r="G53" s="43" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H53" s="43" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="I53" s="45"/>
       <c r="J53" s="42" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="K53" s="46"/>
       <c r="L53" s="46"/>
@@ -4142,7 +4148,7 @@
     </row>
     <row r="54" spans="1:28" ht="29" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B54" s="42">
         <v>20</v>
@@ -4152,17 +4158,17 @@
       <c r="E54" s="43"/>
       <c r="F54" s="43"/>
       <c r="G54" s="43" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H54" s="47" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="I54" s="45"/>
       <c r="J54" s="42" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K54" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L54" s="46"/>
       <c r="M54" s="46"/>
@@ -4184,7 +4190,7 @@
     </row>
     <row r="55" spans="1:28" ht="29" x14ac:dyDescent="0.25">
       <c r="A55" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B55" s="42">
         <v>25</v>
@@ -4194,17 +4200,17 @@
       <c r="E55" s="43"/>
       <c r="F55" s="43"/>
       <c r="G55" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="H55" s="47" t="s">
         <v>193</v>
-      </c>
-      <c r="H55" s="47" t="s">
-        <v>209</v>
       </c>
       <c r="I55" s="45"/>
       <c r="J55" s="42" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K55" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L55" s="46"/>
       <c r="M55" s="46"/>
@@ -4226,7 +4232,7 @@
     </row>
     <row r="56" spans="1:28" ht="29" x14ac:dyDescent="0.25">
       <c r="A56" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B56" s="42">
         <v>20</v>
@@ -4236,17 +4242,17 @@
       <c r="E56" s="43"/>
       <c r="F56" s="43"/>
       <c r="G56" s="43" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H56" s="47" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="I56" s="45"/>
       <c r="J56" s="42" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K56" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L56" s="46"/>
       <c r="M56" s="46"/>
@@ -4268,7 +4274,7 @@
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B57" s="42">
         <v>15</v>
@@ -4278,17 +4284,17 @@
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
       <c r="G57" s="43" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H57" s="43" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="I57" s="45"/>
       <c r="J57" s="42" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="K57" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L57" s="46"/>
       <c r="M57" s="46"/>
@@ -4310,7 +4316,7 @@
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B58" s="42">
         <v>18</v>
@@ -4320,17 +4326,17 @@
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
       <c r="G58" s="43" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H58" s="43" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="I58" s="45"/>
       <c r="J58" s="42" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="K58" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L58" s="46"/>
       <c r="M58" s="46"/>
@@ -4352,7 +4358,7 @@
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B59" s="42">
         <v>25</v>
@@ -4362,17 +4368,17 @@
       <c r="E59" s="43"/>
       <c r="F59" s="43"/>
       <c r="G59" s="43" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H59" s="43" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="I59" s="45"/>
       <c r="J59" s="42" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="K59" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L59" s="46"/>
       <c r="M59" s="46"/>
@@ -4394,7 +4400,7 @@
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="42" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B60" s="42">
         <v>20</v>
@@ -4404,17 +4410,17 @@
       <c r="E60" s="43"/>
       <c r="F60" s="43"/>
       <c r="G60" s="43" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H60" s="43" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="I60" s="45"/>
       <c r="J60" s="42" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="K60" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L60" s="46"/>
       <c r="M60" s="46"/>
@@ -4436,7 +4442,7 @@
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="42" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="B61" s="42">
         <v>13</v>
@@ -4446,17 +4452,17 @@
       <c r="E61" s="43"/>
       <c r="F61" s="43"/>
       <c r="G61" s="43" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="H61" s="43" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="I61" s="45"/>
       <c r="J61" s="42" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="K61" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L61" s="46"/>
       <c r="M61" s="46"/>
@@ -4478,7 +4484,7 @@
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="42" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="B62" s="42">
         <v>12</v>
@@ -4488,17 +4494,17 @@
       <c r="E62" s="43"/>
       <c r="F62" s="43"/>
       <c r="G62" s="43" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="H62" s="43" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="I62" s="45"/>
       <c r="J62" s="42" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="K62" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L62" s="46"/>
       <c r="M62" s="46"/>
@@ -4520,7 +4526,7 @@
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="42" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B63" s="42">
         <v>13</v>
@@ -4530,17 +4536,17 @@
       <c r="E63" s="43"/>
       <c r="F63" s="43"/>
       <c r="G63" s="43" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H63" s="43" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="I63" s="45"/>
       <c r="J63" s="42" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="K63" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L63" s="46"/>
       <c r="M63" s="46"/>
@@ -4562,7 +4568,7 @@
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B64" s="42">
         <v>13</v>
@@ -4572,17 +4578,17 @@
       <c r="E64" s="43"/>
       <c r="F64" s="43"/>
       <c r="G64" s="43" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="H64" s="43" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="I64" s="45"/>
       <c r="J64" s="42" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="K64" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L64" s="46"/>
       <c r="M64" s="46"/>
@@ -4664,7 +4670,7 @@
     </row>
     <row r="67" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="42" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B67" s="42">
         <v>12</v>
@@ -4674,17 +4680,17 @@
       <c r="E67" s="43"/>
       <c r="F67" s="43"/>
       <c r="G67" s="43" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="H67" s="43" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="I67" s="45"/>
       <c r="J67" s="42" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K67" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L67" s="46"/>
       <c r="M67" s="46"/>
@@ -4706,7 +4712,7 @@
     </row>
     <row r="68" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B68" s="13">
         <v>8</v>
@@ -4716,17 +4722,17 @@
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
       <c r="G68" s="25" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K68" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L68" s="16"/>
       <c r="M68" s="16"/>
@@ -4748,7 +4754,7 @@
     </row>
     <row r="69" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B69" s="13">
         <v>9</v>
@@ -4758,17 +4764,17 @@
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
       <c r="G69" s="25" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H69" s="25" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="I69" s="10"/>
       <c r="J69" s="13" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L69" s="16"/>
       <c r="M69" s="16"/>
@@ -4790,7 +4796,7 @@
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B70" s="13">
         <v>9</v>
@@ -4800,17 +4806,17 @@
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
       <c r="G70" s="25" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="H70" s="25" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="I70" s="10"/>
       <c r="J70" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K70" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L70" s="16"/>
       <c r="M70" s="16"/>
@@ -4832,7 +4838,7 @@
     </row>
     <row r="71" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="42" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B71" s="42">
         <v>10</v>
@@ -4842,14 +4848,14 @@
       <c r="E71" s="43"/>
       <c r="F71" s="43"/>
       <c r="G71" s="43" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="H71" s="43" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I71" s="45"/>
       <c r="J71" s="42" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="K71" s="46"/>
       <c r="L71" s="46"/>
@@ -4872,7 +4878,7 @@
     </row>
     <row r="72" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B72" s="13">
         <v>11</v>
@@ -4882,14 +4888,14 @@
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
       <c r="G72" s="25" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H72" s="25" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="I72" s="10"/>
       <c r="J72" s="13" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="K72" s="16"/>
       <c r="L72" s="16"/>
@@ -4912,7 +4918,7 @@
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B73" s="13">
         <v>11</v>
@@ -4922,14 +4928,14 @@
       <c r="E73" s="25"/>
       <c r="F73" s="25"/>
       <c r="G73" s="25" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H73" s="25" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I73" s="10"/>
       <c r="J73" s="13" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="K73" s="16"/>
       <c r="L73" s="16"/>
@@ -4952,7 +4958,7 @@
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74" s="42" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B74" s="42">
         <v>7</v>
@@ -4962,17 +4968,17 @@
       <c r="E74" s="43"/>
       <c r="F74" s="43"/>
       <c r="G74" s="43" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H74" s="43" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I74" s="45"/>
       <c r="J74" s="42" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="K74" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L74" s="46"/>
       <c r="M74" s="46"/>
@@ -5004,7 +5010,7 @@
       <c r="I75" s="45"/>
       <c r="J75" s="42"/>
       <c r="K75" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L75" s="46"/>
       <c r="M75" s="46"/>
@@ -5056,7 +5062,7 @@
     </row>
     <row r="77" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B77" s="13">
         <v>6</v>
@@ -5066,14 +5072,14 @@
       <c r="E77" s="25"/>
       <c r="F77" s="25"/>
       <c r="G77" s="25" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H77" s="25" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="I77" s="10"/>
       <c r="J77" s="13" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="K77" s="16"/>
       <c r="L77" s="16"/>
@@ -5096,7 +5102,7 @@
     </row>
     <row r="78" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B78" s="13">
         <v>6</v>
@@ -5106,14 +5112,14 @@
       <c r="E78" s="25"/>
       <c r="F78" s="25"/>
       <c r="G78" s="25" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H78" s="25" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="I78" s="10"/>
       <c r="J78" s="13" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="K78" s="16"/>
       <c r="L78" s="16"/>
@@ -5136,7 +5142,7 @@
     </row>
     <row r="79" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B79" s="54">
         <v>7</v>
@@ -5146,14 +5152,14 @@
       <c r="E79" s="55"/>
       <c r="F79" s="55"/>
       <c r="G79" s="55" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="H79" s="55" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="I79" s="56"/>
       <c r="J79" s="54" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K79" s="16"/>
       <c r="L79" s="57"/>
@@ -5176,7 +5182,7 @@
     </row>
     <row r="80" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B80" s="13">
         <v>9.5</v>
@@ -5186,17 +5192,17 @@
       <c r="E80" s="25"/>
       <c r="F80" s="25"/>
       <c r="G80" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="I80" s="10"/>
       <c r="J80" s="13" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="K80" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L80" s="16"/>
       <c r="M80" s="16"/>
@@ -5218,7 +5224,7 @@
     </row>
     <row r="81" spans="1:28" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B81" s="10">
         <v>9.5</v>
@@ -5228,22 +5234,22 @@
       <c r="E81" s="58"/>
       <c r="F81" s="58"/>
       <c r="G81" s="25" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="K81" s="59"/>
     </row>
     <row r="82" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B82" s="13">
         <v>9.5</v>
@@ -5253,14 +5259,14 @@
       <c r="E82" s="25"/>
       <c r="F82" s="25"/>
       <c r="G82" s="13" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="I82" s="10"/>
       <c r="J82" s="13" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="K82" s="16"/>
       <c r="L82" s="16"/>
@@ -5283,7 +5289,7 @@
     </row>
     <row r="83" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B83" s="13">
         <v>7</v>
@@ -5293,10 +5299,10 @@
       <c r="E83" s="25"/>
       <c r="F83" s="25"/>
       <c r="G83" s="25" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="H83" s="25" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="I83" s="10"/>
       <c r="J83" s="13"/>
@@ -5321,7 +5327,7 @@
     </row>
     <row r="84" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B84" s="13">
         <v>6</v>
@@ -5331,13 +5337,13 @@
       <c r="E84" s="25"/>
       <c r="F84" s="25"/>
       <c r="G84" s="13" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="10"/>
       <c r="J84" s="13"/>
       <c r="K84" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L84" s="16"/>
       <c r="M84" s="16"/>
@@ -5359,7 +5365,7 @@
     </row>
     <row r="85" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B85" s="13">
         <v>4</v>
@@ -5369,15 +5375,15 @@
       <c r="E85" s="25"/>
       <c r="F85" s="25"/>
       <c r="G85" s="13" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="I85" s="10"/>
       <c r="J85" s="13"/>
       <c r="K85" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L85" s="16"/>
       <c r="M85" s="16"/>
@@ -5399,7 +5405,7 @@
     </row>
     <row r="86" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B86" s="13">
         <v>5.5</v>
@@ -5409,13 +5415,13 @@
       <c r="E86" s="25"/>
       <c r="F86" s="25"/>
       <c r="G86" s="13" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="H86" s="60"/>
       <c r="I86" s="10"/>
       <c r="J86" s="13"/>
       <c r="K86" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L86" s="16"/>
       <c r="M86" s="16"/>
@@ -5437,7 +5443,7 @@
     </row>
     <row r="87" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B87" s="13">
         <v>4.5</v>
@@ -5447,13 +5453,13 @@
       <c r="E87" s="25"/>
       <c r="F87" s="25"/>
       <c r="G87" s="13" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="10"/>
       <c r="J87" s="13"/>
       <c r="K87" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L87" s="16"/>
       <c r="M87" s="16"/>
@@ -5485,7 +5491,7 @@
       <c r="I88" s="13"/>
       <c r="J88" s="13"/>
       <c r="K88" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
@@ -5537,7 +5543,7 @@
     </row>
     <row r="90" spans="1:28" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B90" s="13">
         <v>5</v>
@@ -5547,15 +5553,15 @@
       <c r="E90" s="25"/>
       <c r="F90" s="25"/>
       <c r="G90" s="25" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="H90" s="31" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="I90" s="13"/>
       <c r="J90" s="13"/>
       <c r="K90" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L90" s="16"/>
       <c r="M90" s="16"/>
@@ -5577,7 +5583,7 @@
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B91" s="13">
         <v>12.5</v>
@@ -5587,15 +5593,15 @@
       <c r="E91" s="25"/>
       <c r="F91" s="25"/>
       <c r="G91" s="25" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="H91" s="31" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="16" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L91" s="16"/>
       <c r="M91" s="16"/>
@@ -5617,7 +5623,7 @@
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92" s="42" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B92" s="42">
         <v>5.5</v>
@@ -5627,15 +5633,15 @@
       <c r="E92" s="43"/>
       <c r="F92" s="43"/>
       <c r="G92" s="43" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="H92" s="43" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="I92" s="42"/>
       <c r="J92" s="42"/>
       <c r="K92" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L92" s="46"/>
       <c r="M92" s="46"/>
@@ -5657,7 +5663,7 @@
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93" s="42" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B93" s="42">
         <v>8</v>
@@ -5667,15 +5673,15 @@
       <c r="E93" s="43"/>
       <c r="F93" s="43"/>
       <c r="G93" s="43" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="H93" s="43" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="I93" s="42"/>
       <c r="J93" s="42"/>
       <c r="K93" s="46" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L93" s="46"/>
       <c r="M93" s="46"/>

</xml_diff>

<commit_message>
i dont know what happneed it just works and im puishing it for the sake of it
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://theartsyndicate.sharepoint.com/sites/TheArtSyndicte/Shared Documents/Assets/SRC/Autoscript/TheArtSyndicateMenu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_6600DDEA7A9D30A3CAEF30D588CDE6E726B1BD28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B09E45E-76A1-4DEA-BB03-764B0BFCF4F7}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_6600DDEA7A9D30A3CAEF30D588CDE6E726B1BD28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46C8E2F8-7FD2-4401-A0BC-73BF07854647}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="1440" windowWidth="29040" windowHeight="12510" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,7 +249,7 @@
     <t>Meeting in the Master of Wine program, the winemakers connected over their passion for small batch, terroir driven wine. The thoughtful approach to winemaking and long oak maturation created a layered, ever evolving wine with aromas of lemon curd, fresh yellow apple and baking spices.</t>
   </si>
   <si>
-    <t>Matthew Attalah Wines</t>
+    <t>Matthew Atallah Wines</t>
   </si>
   <si>
     <t>"Block 5, La Femme Nikita"</t>
@@ -258,7 +258,7 @@
     <t>Sauvignon Blanc</t>
   </si>
   <si>
-    <t>Matthew Attalah</t>
+    <t>Matthew Atallah</t>
   </si>
   <si>
     <t>Wth a focus on texture, finesse and balance in all his wines, Matt believes that wines from Orange can stand proudly alongside the world’s best. Taking inspiration from styles of the french Loire Valley, the wine is laden with tropical fruits and herbaceous texture from the extended time in older oak barrels.</t>
@@ -1709,8 +1709,8 @@
   <dimension ref="A1:AB1066"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="E36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="14.45"/>

</xml_diff>